<commit_message>
TS Templates 6.4 to 6.6 08/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE5116A-9F3E-4FDC-9EAC-92C6CB0EEF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187506BC-D136-41C2-92DB-27A7433F5869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7090" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7118" uniqueCount="1222">
   <si>
     <t>Passage</t>
   </si>
@@ -3661,19 +3661,58 @@
   </si>
   <si>
     <t>P[Sh]+S</t>
+  </si>
+  <si>
+    <t>JM-45</t>
+  </si>
+  <si>
+    <t>PS-6.5</t>
+  </si>
+  <si>
+    <t>JM-56</t>
+  </si>
+  <si>
+    <t>PS-4.53</t>
+  </si>
+  <si>
+    <t>GD-83</t>
+  </si>
+  <si>
+    <t>GD-52</t>
+  </si>
+  <si>
+    <t>GD-92</t>
+  </si>
+  <si>
+    <t>GD-78</t>
+  </si>
+  <si>
+    <t>GD-76</t>
+  </si>
+  <si>
+    <t>GD-68</t>
+  </si>
+  <si>
+    <t>JD-40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3863,197 +3902,203 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4337,10 +4382,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2097" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="T2100" sqref="T2100"/>
+      <selection pane="bottomLeft" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10634,7 +10679,9 @@
       <c r="D147" s="30"/>
       <c r="E147" s="24"/>
       <c r="F147" s="24"/>
-      <c r="G147" s="24"/>
+      <c r="G147" s="65" t="s">
+        <v>1215</v>
+      </c>
       <c r="H147" s="24"/>
       <c r="I147" s="59" t="s">
         <v>22</v>
@@ -10674,7 +10721,9 @@
       <c r="D148" s="30"/>
       <c r="E148" s="24"/>
       <c r="F148" s="24"/>
-      <c r="G148" s="24"/>
+      <c r="G148" s="65" t="s">
+        <v>1215</v>
+      </c>
       <c r="H148" s="24"/>
       <c r="I148" s="59" t="s">
         <v>22</v>
@@ -10711,7 +10760,9 @@
     <row r="149" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E149" s="24"/>
       <c r="F149" s="24"/>
-      <c r="G149" s="42"/>
+      <c r="G149" s="65" t="s">
+        <v>1215</v>
+      </c>
       <c r="H149" s="24"/>
       <c r="I149" s="59" t="s">
         <v>22</v>
@@ -14367,8 +14418,12 @@
       </c>
     </row>
     <row r="244" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D244" s="30"/>
-      <c r="E244" s="24"/>
+      <c r="D244" s="66" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E244" s="65" t="s">
+        <v>1211</v>
+      </c>
       <c r="F244" s="24"/>
       <c r="G244" s="24"/>
       <c r="H244" s="61" t="s">
@@ -14407,8 +14462,12 @@
       </c>
     </row>
     <row r="245" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D245" s="30"/>
-      <c r="E245" s="24"/>
+      <c r="D245" s="66" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E245" s="65" t="s">
+        <v>1211</v>
+      </c>
       <c r="F245" s="24"/>
       <c r="G245" s="24"/>
       <c r="H245" s="61" t="s">
@@ -21569,9 +21628,13 @@
     </row>
     <row r="430" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D430" s="30"/>
-      <c r="E430" s="24"/>
+      <c r="E430" s="65" t="s">
+        <v>1213</v>
+      </c>
       <c r="F430" s="24"/>
-      <c r="G430" s="24"/>
+      <c r="G430" s="65" t="s">
+        <v>1216</v>
+      </c>
       <c r="H430" s="61" t="s">
         <v>1176</v>
       </c>
@@ -21609,9 +21672,13 @@
     </row>
     <row r="431" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D431" s="30"/>
-      <c r="E431" s="24"/>
+      <c r="E431" s="65" t="s">
+        <v>1213</v>
+      </c>
       <c r="F431" s="24"/>
-      <c r="G431" s="24"/>
+      <c r="G431" s="65" t="s">
+        <v>1216</v>
+      </c>
       <c r="H431" s="61" t="s">
         <v>1176</v>
       </c>
@@ -21651,7 +21718,9 @@
       <c r="D432" s="30"/>
       <c r="E432" s="24"/>
       <c r="F432" s="24"/>
-      <c r="G432" s="24"/>
+      <c r="G432" s="65" t="s">
+        <v>1216</v>
+      </c>
       <c r="H432" s="61" t="s">
         <v>1176</v>
       </c>
@@ -22386,8 +22455,12 @@
     <row r="451" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D451" s="30"/>
       <c r="E451" s="24"/>
-      <c r="F451" s="24"/>
-      <c r="G451" s="24"/>
+      <c r="F451" s="65" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G451" s="65" t="s">
+        <v>1217</v>
+      </c>
       <c r="H451" s="24"/>
       <c r="I451" s="59" t="s">
         <v>29</v>
@@ -22424,8 +22497,12 @@
     <row r="452" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D452" s="30"/>
       <c r="E452" s="24"/>
-      <c r="F452" s="24"/>
-      <c r="G452" s="24"/>
+      <c r="F452" s="65" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G452" s="65" t="s">
+        <v>1217</v>
+      </c>
       <c r="H452" s="24"/>
       <c r="I452" s="59" t="s">
         <v>29</v>
@@ -22462,8 +22539,12 @@
     <row r="453" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D453" s="30"/>
       <c r="E453" s="24"/>
-      <c r="F453" s="24"/>
-      <c r="G453" s="24"/>
+      <c r="F453" s="65" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G453" s="65" t="s">
+        <v>1217</v>
+      </c>
       <c r="H453" s="24"/>
       <c r="I453" s="59" t="s">
         <v>29</v>
@@ -22501,7 +22582,7 @@
       <c r="D454" s="30"/>
       <c r="E454" s="24"/>
       <c r="F454" s="24"/>
-      <c r="G454" s="24"/>
+      <c r="G454" s="65"/>
       <c r="H454" s="24"/>
       <c r="I454" s="59" t="s">
         <v>29</v>
@@ -40276,7 +40357,9 @@
     <row r="921" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E921" s="24"/>
       <c r="F921" s="24"/>
-      <c r="G921" s="24"/>
+      <c r="G921" s="65" t="s">
+        <v>1219</v>
+      </c>
       <c r="H921" s="61" t="s">
         <v>1189</v>
       </c>
@@ -40320,7 +40403,9 @@
       </c>
       <c r="E922" s="24"/>
       <c r="F922" s="24"/>
-      <c r="G922" s="24"/>
+      <c r="G922" s="65" t="s">
+        <v>1219</v>
+      </c>
       <c r="H922" s="61" t="s">
         <v>1189</v>
       </c>
@@ -40359,7 +40444,9 @@
     <row r="923" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E923" s="24"/>
       <c r="F923" s="24"/>
-      <c r="G923" s="24"/>
+      <c r="G923" s="65" t="s">
+        <v>1219</v>
+      </c>
       <c r="H923" s="61" t="s">
         <v>1189</v>
       </c>
@@ -64279,7 +64366,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="1553" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1553" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1553" s="24"/>
       <c r="F1553" s="24"/>
       <c r="G1553" s="24"/>
@@ -64316,7 +64403,7 @@
       <c r="U1553" s="8"/>
       <c r="V1553" s="56"/>
     </row>
-    <row r="1554" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1554" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1554" s="24"/>
       <c r="F1554" s="24"/>
       <c r="G1554" s="24"/>
@@ -64353,7 +64440,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="1555" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1555" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1555" s="24"/>
       <c r="F1555" s="24"/>
       <c r="G1555" s="24"/>
@@ -64390,7 +64477,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="1556" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1556" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1556" s="24"/>
       <c r="F1556" s="24"/>
       <c r="G1556" s="24"/>
@@ -64427,7 +64514,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="1557" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1557" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1557" s="24"/>
       <c r="F1557" s="24"/>
       <c r="G1557" s="24"/>
@@ -64464,7 +64551,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="1558" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1558" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1558" s="24"/>
       <c r="F1558" s="24"/>
       <c r="G1558" s="24"/>
@@ -64501,7 +64588,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="1559" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1559" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1559" s="24"/>
       <c r="F1559" s="24"/>
       <c r="G1559" s="24"/>
@@ -64538,10 +64625,17 @@
         <v>685</v>
       </c>
     </row>
-    <row r="1560" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="E1560" s="24"/>
-      <c r="F1560" s="24"/>
-      <c r="G1560" s="24"/>
+    <row r="1560" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D1560" s="66" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E1560" s="65"/>
+      <c r="F1560" s="65" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1560" s="65" t="s">
+        <v>1220</v>
+      </c>
       <c r="H1560" s="24"/>
       <c r="I1560" s="59" t="s">
         <v>50</v>
@@ -64575,10 +64669,17 @@
         <v>686</v>
       </c>
     </row>
-    <row r="1561" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="E1561" s="24"/>
-      <c r="F1561" s="24"/>
-      <c r="G1561" s="24"/>
+    <row r="1561" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D1561" s="66" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E1561" s="65"/>
+      <c r="F1561" s="65" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G1561" s="65" t="s">
+        <v>1220</v>
+      </c>
       <c r="H1561" s="24"/>
       <c r="I1561" s="59" t="s">
         <v>50</v>
@@ -64612,10 +64713,12 @@
         <v>687</v>
       </c>
     </row>
-    <row r="1562" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1562" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1562" s="24"/>
       <c r="F1562" s="24"/>
-      <c r="G1562" s="24"/>
+      <c r="G1562" s="65" t="s">
+        <v>1220</v>
+      </c>
       <c r="H1562" s="24"/>
       <c r="I1562" s="59" t="s">
         <v>50</v>
@@ -64649,7 +64752,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="1563" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1563" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1563" s="24"/>
       <c r="F1563" s="24"/>
       <c r="G1563" s="24"/>
@@ -64686,7 +64789,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="1564" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1564" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1564" s="24"/>
       <c r="F1564" s="24"/>
       <c r="G1564" s="24"/>
@@ -64723,7 +64826,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="1565" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1565" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1565" s="24"/>
       <c r="F1565" s="24"/>
       <c r="G1565" s="24"/>
@@ -64760,7 +64863,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="1566" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1566" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1566" s="24"/>
       <c r="F1566" s="24"/>
       <c r="G1566" s="24"/>
@@ -64797,7 +64900,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="1567" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1567" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1567" s="23"/>
       <c r="F1567" s="24"/>
       <c r="G1567" s="24"/>
@@ -64836,7 +64939,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="1568" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1568" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1568" s="24"/>
       <c r="F1568" s="24"/>
       <c r="G1568" s="24"/>

</xml_diff>

<commit_message>
Update TS 6.5 Padam Input Template.xlsx
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9BA8C1-3657-4B4F-AABF-6CDF793C0F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C6FC7-5AC7-480E-83D1-C082BE4FC97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5543" uniqueCount="1228">
   <si>
     <t>Passage</t>
   </si>
@@ -3674,9 +3674,6 @@
     <t>agnA(3),i</t>
   </si>
   <si>
-    <t>P{Sh]%S</t>
-  </si>
-  <si>
     <t>N[r]+S[r]</t>
   </si>
   <si>
@@ -3717,6 +3714,12 @@
   </si>
   <si>
     <t>S%P[Sh]</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prAqNaH </t>
   </si>
 </sst>
 </file>
@@ -3866,7 +3869,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3894,6 +3897,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3925,7 +3934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4097,11 +4106,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4385,10 +4397,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2147" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2138" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2150" sqref="N2150"/>
+      <selection pane="bottomLeft" activeCell="N2135" sqref="N2135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5549,7 +5561,7 @@
         <v>76</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="45"/>
@@ -9830,7 +9842,7 @@
         <v>70</v>
       </c>
       <c r="T135" s="8" t="s">
-        <v>1212</v>
+        <v>1219</v>
       </c>
       <c r="U135" s="8"/>
       <c r="V135" s="45"/>
@@ -10367,7 +10379,7 @@
         <v>76</v>
       </c>
       <c r="T151" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U151" s="8"/>
       <c r="V151" s="45" t="s">
@@ -10842,7 +10854,9 @@
       <c r="R165" s="8"/>
       <c r="S165" s="8"/>
       <c r="T165" s="8"/>
-      <c r="U165" s="8"/>
+      <c r="U165" s="8" t="s">
+        <v>1226</v>
+      </c>
       <c r="V165" s="45" t="s">
         <v>977</v>
       </c>
@@ -11965,7 +11979,7 @@
         <v>73</v>
       </c>
       <c r="T199" s="8" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U199" s="8"/>
       <c r="V199" s="45"/>
@@ -13697,7 +13711,9 @@
       <c r="R250" s="8"/>
       <c r="S250" s="8"/>
       <c r="T250" s="8"/>
-      <c r="U250" s="8"/>
+      <c r="U250" s="8" t="s">
+        <v>1226</v>
+      </c>
       <c r="V250" s="45"/>
     </row>
     <row r="251" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14919,8 +14935,8 @@
         <f t="shared" si="14"/>
         <v>53</v>
       </c>
-      <c r="N287" s="45" t="s">
-        <v>257</v>
+      <c r="N287" s="60" t="s">
+        <v>1227</v>
       </c>
       <c r="O287" s="8" t="s">
         <v>62</v>
@@ -20446,7 +20462,7 @@
         <v>76</v>
       </c>
       <c r="T451" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U451" s="8"/>
       <c r="V451" s="45"/>
@@ -21232,7 +21248,7 @@
         <v>76</v>
       </c>
       <c r="T474" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U474" s="8"/>
       <c r="V474" s="45"/>
@@ -21908,7 +21924,7 @@
         <v>76</v>
       </c>
       <c r="T494" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U494" s="8"/>
       <c r="V494" s="45"/>
@@ -25849,7 +25865,7 @@
         <v>53</v>
       </c>
       <c r="N610" s="51" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="O610" s="7"/>
       <c r="P610" s="8"/>
@@ -28742,7 +28758,7 @@
     </row>
     <row r="699" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A699" s="8" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="I699" s="48" t="s">
         <v>35</v>
@@ -32487,7 +32503,7 @@
         <f t="shared" si="38"/>
         <v>178</v>
       </c>
-      <c r="N815" s="56" t="s">
+      <c r="N815" s="45" t="s">
         <v>292</v>
       </c>
       <c r="O815" s="7"/>
@@ -35740,7 +35756,7 @@
         <v>76</v>
       </c>
       <c r="T917" s="8" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="U917" s="8"/>
       <c r="V917" s="45"/>
@@ -41406,7 +41422,7 @@
         <f t="shared" ref="M1092:M1155" si="53">+M1091+1</f>
         <v>277</v>
       </c>
-      <c r="N1092" s="45" t="s">
+      <c r="N1092" s="57" t="s">
         <v>612</v>
       </c>
       <c r="O1092" s="8" t="s">
@@ -43497,7 +43513,7 @@
         <v>81</v>
       </c>
       <c r="T1156" s="8" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="V1156" s="45"/>
     </row>
@@ -46866,7 +46882,7 @@
         <f t="shared" si="59"/>
         <v>169</v>
       </c>
-      <c r="N1261" s="57" t="s">
+      <c r="N1261" s="61" t="s">
         <v>191</v>
       </c>
       <c r="O1261" s="7"/>
@@ -49368,7 +49384,7 @@
         <f t="shared" si="62"/>
         <v>75</v>
       </c>
-      <c r="N1336" s="59" t="s">
+      <c r="N1336" s="45" t="s">
         <v>127</v>
       </c>
       <c r="O1336" s="8" t="s">
@@ -60430,7 +60446,7 @@
         <v>76</v>
       </c>
       <c r="T1694" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="V1694" s="45"/>
     </row>
@@ -62337,17 +62353,17 @@
         <f t="shared" si="83"/>
         <v>200</v>
       </c>
-      <c r="N1769" s="60" t="s">
+      <c r="N1769" s="59" t="s">
         <v>842</v>
       </c>
       <c r="P1769" s="8" t="s">
         <v>63</v>
       </c>
       <c r="S1769" s="8" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="T1769" s="8" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="V1769" s="46" t="s">
         <v>1173</v>
@@ -63160,10 +63176,10 @@
       <c r="N1800" s="45" t="s">
         <v>859</v>
       </c>
-      <c r="S1800" s="1" t="s">
+      <c r="S1800" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="T1800" s="1" t="s">
+      <c r="T1800" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V1800" s="45"/>
@@ -64590,10 +64606,10 @@
         <v>65</v>
       </c>
       <c r="S1857" s="8" t="s">
+        <v>1216</v>
+      </c>
+      <c r="T1857" s="8" t="s">
         <v>1217</v>
-      </c>
-      <c r="T1857" s="8" t="s">
-        <v>1218</v>
       </c>
       <c r="V1857" s="45"/>
     </row>
@@ -66638,7 +66654,7 @@
         <f t="shared" si="92"/>
         <v>168</v>
       </c>
-      <c r="N1937" s="59" t="s">
+      <c r="N1937" s="45" t="s">
         <v>286</v>
       </c>
       <c r="P1937" s="8" t="s">
@@ -66699,7 +66715,7 @@
         <v>81</v>
       </c>
       <c r="T1939" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="V1939" s="45"/>
     </row>
@@ -67193,7 +67209,7 @@
         <v>76</v>
       </c>
       <c r="T1959" s="8" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="V1959" s="45"/>
     </row>
@@ -67416,7 +67432,7 @@
         <v>76</v>
       </c>
       <c r="T1967" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="V1967" s="45" t="s">
         <v>975</v>
@@ -67918,7 +67934,7 @@
         <v>76</v>
       </c>
       <c r="T1987" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="V1987" s="45"/>
     </row>
@@ -68051,7 +68067,7 @@
         <v>76</v>
       </c>
       <c r="T1992" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="V1992" s="45"/>
     </row>
@@ -68554,7 +68570,7 @@
         <v>76</v>
       </c>
       <c r="T2012" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="V2012" s="45"/>
     </row>
@@ -69186,7 +69202,7 @@
         <f t="shared" si="94"/>
         <v>100</v>
       </c>
-      <c r="N2037" s="57" t="s">
+      <c r="N2037" s="61" t="s">
         <v>148</v>
       </c>
       <c r="V2037" s="45"/>
@@ -70432,7 +70448,7 @@
         <v>150</v>
       </c>
       <c r="N2087" s="51" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="V2087" s="45"/>
     </row>
@@ -70801,7 +70817,7 @@
         <v>70</v>
       </c>
       <c r="T2101" s="8" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="V2101" s="45"/>
     </row>
@@ -71084,10 +71100,10 @@
         <v>65</v>
       </c>
       <c r="S2112" s="8" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="T2112" s="8" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="V2112" s="45"/>
     </row>

</xml_diff>

<commit_message>
TS 6.4 to 6.6 Padam Template edits - 27/04/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C6FC7-5AC7-480E-83D1-C082BE4FC97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9203C2B8-4C56-4AC0-860F-2F500FA15F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5543" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5542" uniqueCount="1228">
   <si>
     <t>Passage</t>
   </si>
@@ -4106,14 +4098,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4397,10 +4389,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2138" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2135" sqref="N2135"/>
+      <selection pane="bottomLeft" activeCell="O396" sqref="O396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -14935,7 +14927,7 @@
         <f t="shared" si="14"/>
         <v>53</v>
       </c>
-      <c r="N287" s="60" t="s">
+      <c r="N287" s="59" t="s">
         <v>1227</v>
       </c>
       <c r="O287" s="8" t="s">
@@ -46882,7 +46874,7 @@
         <f t="shared" si="59"/>
         <v>169</v>
       </c>
-      <c r="N1261" s="61" t="s">
+      <c r="N1261" s="45" t="s">
         <v>191</v>
       </c>
       <c r="O1261" s="7"/>
@@ -47515,7 +47507,9 @@
       <c r="N1280" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="O1280" s="8"/>
+      <c r="O1280" s="60" t="s">
+        <v>65</v>
+      </c>
       <c r="P1280" s="8"/>
       <c r="Q1280" s="8"/>
       <c r="R1280" s="8"/>
@@ -62353,7 +62347,7 @@
         <f t="shared" si="83"/>
         <v>200</v>
       </c>
-      <c r="N1769" s="59" t="s">
+      <c r="N1769" s="61" t="s">
         <v>842</v>
       </c>
       <c r="P1769" s="8" t="s">
@@ -66711,12 +66705,6 @@
       <c r="N1939" s="45" t="s">
         <v>907</v>
       </c>
-      <c r="S1939" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="T1939" s="1" t="s">
-        <v>1214</v>
-      </c>
       <c r="V1939" s="45"/>
     </row>
     <row r="1940" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69202,7 +69190,7 @@
         <f t="shared" si="94"/>
         <v>100</v>
       </c>
-      <c r="N2037" s="61" t="s">
+      <c r="N2037" s="45" t="s">
         <v>148</v>
       </c>
       <c r="V2037" s="45"/>

</xml_diff>

<commit_message>
nmv 31 10 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9203C2B8-4C56-4AC0-860F-2F500FA15F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5319FED2-1119-4845-ACF0-1F78349F803C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 6.5" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 6.5'!$C$1:$V$2151</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5542" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5544" uniqueCount="1228">
   <si>
     <t>Passage</t>
   </si>
@@ -3693,18 +3693,12 @@
     <t>S[s]+P[S]</t>
   </si>
   <si>
-    <t>praqtya~g~g</t>
-  </si>
-  <si>
     <t>sa(gg)skurute</t>
   </si>
   <si>
     <t>S[r]+N[r]+P[r]</t>
   </si>
   <si>
-    <t xml:space="preserve">viShva~g~g# </t>
-  </si>
-  <si>
     <t>S%P[Sh]</t>
   </si>
   <si>
@@ -3712,13 +3706,19 @@
   </si>
   <si>
     <t xml:space="preserve">prAqNaH </t>
+  </si>
+  <si>
+    <t>praqtya~g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">viShva~g# </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3860,6 +3860,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3882,12 +3888,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3895,6 +3895,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3926,7 +3932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4094,17 +4100,50 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4389,10 +4428,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A678" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O396" sqref="O396"/>
+      <selection pane="bottomLeft" activeCell="I688" sqref="I688:S688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10847,7 +10886,7 @@
       <c r="S165" s="8"/>
       <c r="T165" s="8"/>
       <c r="U165" s="8" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="V165" s="45" t="s">
         <v>977</v>
@@ -13704,7 +13743,7 @@
       <c r="S250" s="8"/>
       <c r="T250" s="8"/>
       <c r="U250" s="8" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="V250" s="45"/>
     </row>
@@ -14927,8 +14966,8 @@
         <f t="shared" si="14"/>
         <v>53</v>
       </c>
-      <c r="N287" s="59" t="s">
-        <v>1227</v>
+      <c r="N287" s="45" t="s">
+        <v>1225</v>
       </c>
       <c r="O287" s="8" t="s">
         <v>62</v>
@@ -17795,7 +17834,7 @@
         <f t="shared" si="17"/>
         <v>139</v>
       </c>
-      <c r="N373" s="56" t="s">
+      <c r="N373" s="45" t="s">
         <v>292</v>
       </c>
       <c r="O373" s="8"/>
@@ -24085,7 +24124,7 @@
         <f t="shared" si="26"/>
         <v>184</v>
       </c>
-      <c r="N557" s="57" t="s">
+      <c r="N557" s="45" t="s">
         <v>350</v>
       </c>
       <c r="O557" s="7"/>
@@ -24718,7 +24757,7 @@
         <f t="shared" si="26"/>
         <v>19</v>
       </c>
-      <c r="N576" s="58" t="s">
+      <c r="N576" s="57" t="s">
         <v>127</v>
       </c>
       <c r="O576" s="8" t="s">
@@ -25856,8 +25895,8 @@
         <f t="shared" si="29"/>
         <v>53</v>
       </c>
-      <c r="N610" s="51" t="s">
-        <v>1221</v>
+      <c r="N610" s="46" t="s">
+        <v>1226</v>
       </c>
       <c r="O610" s="7"/>
       <c r="P610" s="8"/>
@@ -26120,7 +26159,9 @@
       <c r="N618" s="45" t="s">
         <v>411</v>
       </c>
-      <c r="O618" s="7"/>
+      <c r="O618" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="P618" s="8"/>
       <c r="Q618" s="8"/>
       <c r="R618" s="8"/>
@@ -28405,31 +28446,31 @@
       <c r="V687" s="45"/>
     </row>
     <row r="688" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I688" s="48" t="s">
+      <c r="I688" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="J688" s="9">
+      <c r="J688" s="61">
         <v>16</v>
       </c>
-      <c r="K688" s="6">
+      <c r="K688" s="62">
         <f t="shared" si="30"/>
         <v>687</v>
       </c>
-      <c r="L688" s="6">
+      <c r="L688" s="62">
         <v>1</v>
       </c>
-      <c r="M688" s="6">
+      <c r="M688" s="62">
         <f t="shared" si="32"/>
         <v>51</v>
       </c>
-      <c r="N688" s="45" t="s">
+      <c r="N688" s="63" t="s">
         <v>434</v>
       </c>
-      <c r="O688" s="7"/>
-      <c r="P688" s="8"/>
-      <c r="Q688" s="8"/>
-      <c r="R688" s="8"/>
-      <c r="S688" s="8"/>
+      <c r="O688" s="64"/>
+      <c r="P688" s="65"/>
+      <c r="Q688" s="65"/>
+      <c r="R688" s="65"/>
+      <c r="S688" s="65"/>
       <c r="T688" s="8"/>
       <c r="U688" s="8"/>
       <c r="V688" s="45"/>
@@ -28734,7 +28775,7 @@
         <f t="shared" si="32"/>
         <v>61</v>
       </c>
-      <c r="N698" s="51" t="s">
+      <c r="N698" s="59" t="s">
         <v>439</v>
       </c>
       <c r="O698" s="8" t="s">
@@ -28750,7 +28791,7 @@
     </row>
     <row r="699" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A699" s="8" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="I699" s="48" t="s">
         <v>35</v>
@@ -28770,7 +28811,7 @@
         <f t="shared" si="32"/>
         <v>62</v>
       </c>
-      <c r="N699" s="51" t="s">
+      <c r="N699" s="59" t="s">
         <v>364</v>
       </c>
       <c r="O699" s="7"/>
@@ -35748,7 +35789,7 @@
         <v>76</v>
       </c>
       <c r="T917" s="8" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="U917" s="8"/>
       <c r="V917" s="45"/>
@@ -36396,7 +36437,9 @@
       <c r="N936" s="45" t="s">
         <v>411</v>
       </c>
-      <c r="O936" s="7"/>
+      <c r="O936" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="P936" s="8"/>
       <c r="Q936" s="8"/>
       <c r="R936" s="8"/>
@@ -38900,33 +38943,33 @@
       <c r="V1014" s="45"/>
     </row>
     <row r="1015" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1015" s="48" t="s">
+      <c r="I1015" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="J1015" s="9">
+      <c r="J1015" s="67">
         <v>21</v>
       </c>
-      <c r="K1015" s="6">
+      <c r="K1015" s="68">
         <f t="shared" si="45"/>
         <v>1014</v>
       </c>
-      <c r="L1015" s="6">
+      <c r="L1015" s="68">
         <f t="shared" si="46"/>
         <v>50</v>
       </c>
-      <c r="M1015" s="6">
+      <c r="M1015" s="68">
         <f t="shared" si="47"/>
         <v>200</v>
       </c>
-      <c r="N1015" s="45" t="s">
+      <c r="N1015" s="69" t="s">
         <v>292</v>
       </c>
-      <c r="O1015" s="7"/>
-      <c r="P1015" s="8"/>
-      <c r="Q1015" s="8"/>
-      <c r="R1015" s="8"/>
-      <c r="S1015" s="8"/>
-      <c r="T1015" s="8"/>
+      <c r="O1015" s="70"/>
+      <c r="P1015" s="71"/>
+      <c r="Q1015" s="71"/>
+      <c r="R1015" s="71"/>
+      <c r="S1015" s="71"/>
+      <c r="T1015" s="71"/>
       <c r="U1015" s="8"/>
       <c r="V1015" s="45"/>
     </row>
@@ -41414,7 +41457,7 @@
         <f t="shared" ref="M1092:M1155" si="53">+M1091+1</f>
         <v>277</v>
       </c>
-      <c r="N1092" s="57" t="s">
+      <c r="N1092" s="69" t="s">
         <v>612</v>
       </c>
       <c r="O1092" s="8" t="s">
@@ -47507,7 +47550,7 @@
       <c r="N1280" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="O1280" s="60" t="s">
+      <c r="O1280" s="58" t="s">
         <v>65</v>
       </c>
       <c r="P1280" s="8"/>
@@ -62347,7 +62390,7 @@
         <f t="shared" si="83"/>
         <v>200</v>
       </c>
-      <c r="N1769" s="61" t="s">
+      <c r="N1769" s="46" t="s">
         <v>842</v>
       </c>
       <c r="P1769" s="8" t="s">
@@ -70435,8 +70478,8 @@
         <f t="shared" si="98"/>
         <v>150</v>
       </c>
-      <c r="N2087" s="51" t="s">
-        <v>1224</v>
+      <c r="N2087" s="72" t="s">
+        <v>1227</v>
       </c>
       <c r="V2087" s="45"/>
     </row>
@@ -71091,7 +71134,7 @@
         <v>1216</v>
       </c>
       <c r="T2112" s="8" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="V2112" s="45"/>
     </row>
@@ -72057,7 +72100,7 @@
         <f t="shared" si="101"/>
         <v>214</v>
       </c>
-      <c r="N2151" s="57" t="s">
+      <c r="N2151" s="56" t="s">
         <v>961</v>
       </c>
       <c r="O2151" s="8" t="s">

</xml_diff>

<commit_message>
nmv 16 12 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC25224-748A-43DD-B97B-A4BB3753FD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88781A54-C7E3-4EB5-9D75-C446E2AA6FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2647,9 +2647,6 @@
   </si>
   <si>
     <t xml:space="preserve">vAqyaqvye#na </t>
-  </si>
-  <si>
-    <t xml:space="preserve">gaBe#rNa </t>
   </si>
   <si>
     <t xml:space="preserve">avi#j~jAtena </t>
@@ -3788,6 +3785,9 @@
   </si>
   <si>
     <t xml:space="preserve">iqndriqyAqvaqH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">garBe#Na </t>
   </si>
 </sst>
 </file>
@@ -4536,9 +4536,9 @@
   <dimension ref="A1:V2151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1401" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1863" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1410" sqref="N1410"/>
+      <selection pane="bottomLeft" activeCell="N1870" sqref="N1870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5333,7 +5333,7 @@
         <v>7</v>
       </c>
       <c r="N8" s="45" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="17"/>
@@ -5423,7 +5423,7 @@
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
       <c r="V10" s="45" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -5699,7 +5699,7 @@
         <v>76</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="45"/>
@@ -8410,7 +8410,7 @@
       <c r="T89" s="17"/>
       <c r="U89" s="17"/>
       <c r="V89" s="45" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="90" spans="1:22" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9072,7 +9072,7 @@
       <c r="T109" s="8"/>
       <c r="U109" s="8"/>
       <c r="V109" s="45" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="110" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9732,7 +9732,7 @@
       <c r="T128" s="8"/>
       <c r="U128" s="8"/>
       <c r="V128" s="45" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="129" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9906,7 +9906,7 @@
       <c r="T133" s="8"/>
       <c r="U133" s="8"/>
       <c r="V133" s="45" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="134" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9980,7 +9980,7 @@
         <v>70</v>
       </c>
       <c r="T135" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U135" s="8"/>
       <c r="V135" s="45"/>
@@ -10378,7 +10378,7 @@
       <c r="T147" s="8"/>
       <c r="U147" s="8"/>
       <c r="V147" s="45" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="148" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10517,11 +10517,11 @@
         <v>76</v>
       </c>
       <c r="T151" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="U151" s="8"/>
       <c r="V151" s="45" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="152" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10629,7 +10629,7 @@
       <c r="T154" s="8"/>
       <c r="U154" s="8"/>
       <c r="V154" s="45" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="155" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10993,10 +10993,10 @@
       <c r="S165" s="8"/>
       <c r="T165" s="8"/>
       <c r="U165" s="8" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="V165" s="45" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="166" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11848,7 +11848,7 @@
       <c r="T191" s="8"/>
       <c r="U191" s="8"/>
       <c r="V191" s="45" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="192" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11980,7 +11980,7 @@
       <c r="T195" s="8"/>
       <c r="U195" s="8"/>
       <c r="V195" s="45" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="196" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12048,7 +12048,7 @@
       <c r="T197" s="8"/>
       <c r="U197" s="8"/>
       <c r="V197" s="45" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="198" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12117,7 +12117,7 @@
         <v>73</v>
       </c>
       <c r="T199" s="8" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="U199" s="8"/>
       <c r="V199" s="45"/>
@@ -12293,7 +12293,7 @@
       <c r="T204" s="8"/>
       <c r="U204" s="8"/>
       <c r="V204" s="45" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="205" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
       <c r="T209" s="8"/>
       <c r="U209" s="8"/>
       <c r="V209" s="45" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="210" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12598,7 +12598,7 @@
       <c r="T213" s="8"/>
       <c r="U213" s="8"/>
       <c r="V213" s="45" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="214" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12800,7 +12800,7 @@
       <c r="T219" s="8"/>
       <c r="U219" s="8"/>
       <c r="V219" s="45" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="220" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12964,7 +12964,7 @@
       <c r="T224" s="8"/>
       <c r="U224" s="8"/>
       <c r="V224" s="45" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="225" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13096,7 +13096,7 @@
       <c r="T228" s="8"/>
       <c r="U228" s="8"/>
       <c r="V228" s="45" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="229" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13262,7 +13262,7 @@
       <c r="T233" s="8"/>
       <c r="U233" s="8"/>
       <c r="V233" s="45" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="234" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13298,7 +13298,7 @@
       <c r="T234" s="8"/>
       <c r="U234" s="8"/>
       <c r="V234" s="45" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="235" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13526,7 +13526,7 @@
       <c r="T241" s="8"/>
       <c r="U241" s="8"/>
       <c r="V241" s="45" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="242" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13715,7 +13715,7 @@
       <c r="T246" s="8"/>
       <c r="U246" s="8"/>
       <c r="V246" s="45" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="247" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13752,7 +13752,7 @@
       <c r="T247" s="8"/>
       <c r="U247" s="8"/>
       <c r="V247" s="45" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="248" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13850,7 +13850,7 @@
       <c r="S250" s="8"/>
       <c r="T250" s="8"/>
       <c r="U250" s="8" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="V250" s="45"/>
     </row>
@@ -14473,7 +14473,7 @@
       <c r="T269" s="8"/>
       <c r="U269" s="8"/>
       <c r="V269" s="45" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="270" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14607,7 +14607,7 @@
       <c r="T273" s="8"/>
       <c r="U273" s="8"/>
       <c r="V273" s="45" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="274" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15074,7 +15074,7 @@
         <v>53</v>
       </c>
       <c r="N287" s="45" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O287" s="8" t="s">
         <v>62</v>
@@ -15086,7 +15086,7 @@
       <c r="T287" s="8"/>
       <c r="U287" s="8"/>
       <c r="V287" s="45" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="288" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15156,7 +15156,7 @@
       <c r="T289" s="8"/>
       <c r="U289" s="8"/>
       <c r="V289" s="45" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="290" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15193,7 +15193,7 @@
       <c r="T290" s="8"/>
       <c r="U290" s="8"/>
       <c r="V290" s="45" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="291" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15326,7 +15326,7 @@
       <c r="T294" s="8"/>
       <c r="U294" s="8"/>
       <c r="V294" s="45" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="295" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15494,7 +15494,7 @@
       <c r="T299" s="8"/>
       <c r="U299" s="8"/>
       <c r="V299" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="300" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15532,7 +15532,7 @@
       <c r="T300" s="8"/>
       <c r="U300" s="8"/>
       <c r="V300" s="45" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="301" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15698,7 +15698,7 @@
       <c r="T305" s="8"/>
       <c r="U305" s="8"/>
       <c r="V305" s="45" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="306" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15766,7 +15766,7 @@
       <c r="T307" s="8"/>
       <c r="U307" s="8"/>
       <c r="V307" s="45" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="308" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15995,7 +15995,7 @@
       <c r="T314" s="8"/>
       <c r="U314" s="8"/>
       <c r="V314" s="45" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="315" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -16095,7 +16095,7 @@
       <c r="T317" s="8"/>
       <c r="U317" s="8"/>
       <c r="V317" s="45" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="318" spans="2:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -16483,7 +16483,7 @@
       <c r="T329" s="8"/>
       <c r="U329" s="8"/>
       <c r="V329" s="45" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="330" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -16551,7 +16551,7 @@
       <c r="T331" s="8"/>
       <c r="U331" s="8"/>
       <c r="V331" s="45" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="332" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -16810,7 +16810,7 @@
       <c r="T339" s="8"/>
       <c r="U339" s="8"/>
       <c r="V339" s="45" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="340" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17070,7 +17070,7 @@
       <c r="T347" s="8"/>
       <c r="U347" s="8"/>
       <c r="V347" s="45" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="348" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17298,7 +17298,7 @@
       <c r="T354" s="8"/>
       <c r="U354" s="8"/>
       <c r="V354" s="45" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="355" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17335,7 +17335,7 @@
       <c r="T355" s="8"/>
       <c r="U355" s="8"/>
       <c r="V355" s="45" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="356" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17438,7 +17438,7 @@
       <c r="T358" s="8"/>
       <c r="U358" s="8"/>
       <c r="V358" s="45" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="359" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17574,7 +17574,7 @@
       <c r="T362" s="8"/>
       <c r="U362" s="8"/>
       <c r="V362" s="45" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="363" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17745,7 +17745,7 @@
       <c r="T367" s="8"/>
       <c r="U367" s="8"/>
       <c r="V367" s="45" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="368" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17815,7 +17815,7 @@
       <c r="T369" s="8"/>
       <c r="U369" s="8"/>
       <c r="V369" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="370" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17852,7 +17852,7 @@
       <c r="T370" s="8"/>
       <c r="U370" s="8"/>
       <c r="V370" s="45" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="371" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17954,7 +17954,7 @@
       <c r="T373" s="8"/>
       <c r="U373" s="8"/>
       <c r="V373" s="45" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="374" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18084,7 +18084,7 @@
       <c r="T377" s="8"/>
       <c r="U377" s="8"/>
       <c r="V377" s="45" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="378" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18312,7 +18312,7 @@
       <c r="T384" s="8"/>
       <c r="U384" s="8"/>
       <c r="V384" s="45" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="385" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18412,7 +18412,7 @@
       <c r="T387" s="8"/>
       <c r="U387" s="8"/>
       <c r="V387" s="45" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="388" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18480,7 +18480,7 @@
       <c r="T389" s="8"/>
       <c r="U389" s="8"/>
       <c r="V389" s="45" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="390" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18653,7 +18653,7 @@
       <c r="T394" s="8"/>
       <c r="U394" s="8"/>
       <c r="V394" s="45" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="395" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18866,7 +18866,7 @@
       <c r="T400" s="8"/>
       <c r="U400" s="8"/>
       <c r="V400" s="45" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="401" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18934,7 +18934,7 @@
       <c r="T402" s="8"/>
       <c r="U402" s="8"/>
       <c r="V402" s="45" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="403" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19002,7 +19002,7 @@
       <c r="T404" s="8"/>
       <c r="U404" s="8"/>
       <c r="V404" s="45" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="405" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19166,7 +19166,7 @@
       <c r="T409" s="8"/>
       <c r="U409" s="8"/>
       <c r="V409" s="45" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="410" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19202,7 +19202,7 @@
       <c r="T410" s="8"/>
       <c r="U410" s="8"/>
       <c r="V410" s="45" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="411" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19238,7 +19238,7 @@
       <c r="T411" s="8"/>
       <c r="U411" s="8"/>
       <c r="V411" s="45" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="412" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19326,7 +19326,7 @@
         <v>41</v>
       </c>
       <c r="N414" s="46" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="O414" s="7" t="s">
         <v>64</v>
@@ -19338,7 +19338,7 @@
       <c r="T414" s="8"/>
       <c r="U414" s="8"/>
       <c r="V414" s="45" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="415" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19406,7 +19406,7 @@
       <c r="T416" s="8"/>
       <c r="U416" s="8"/>
       <c r="V416" s="45" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="417" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19474,7 +19474,7 @@
       <c r="T418" s="8"/>
       <c r="U418" s="8"/>
       <c r="V418" s="45" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="419" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19510,7 +19510,7 @@
       <c r="T419" s="8"/>
       <c r="U419" s="8"/>
       <c r="V419" s="45" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="420" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19546,7 +19546,7 @@
       <c r="T420" s="8"/>
       <c r="U420" s="8"/>
       <c r="V420" s="45" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="421" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19582,7 +19582,7 @@
       <c r="T421" s="8"/>
       <c r="U421" s="8"/>
       <c r="V421" s="45" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="422" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19845,7 +19845,7 @@
     </row>
     <row r="430" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A430" s="60" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B430" s="55"/>
       <c r="C430" s="55"/>
@@ -20337,7 +20337,7 @@
       <c r="T443" s="8"/>
       <c r="U443" s="8"/>
       <c r="V443" s="45" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="444" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20437,7 +20437,7 @@
       <c r="T446" s="8"/>
       <c r="U446" s="8"/>
       <c r="V446" s="45" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="447" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20605,7 +20605,7 @@
         <v>76</v>
       </c>
       <c r="T451" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="U451" s="8"/>
       <c r="V451" s="45"/>
@@ -20720,7 +20720,7 @@
       <c r="T454" s="8"/>
       <c r="U454" s="8"/>
       <c r="V454" s="45" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="455" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20821,7 +20821,7 @@
     </row>
     <row r="458" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A458" s="60" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D458" s="24"/>
       <c r="I458" s="48" t="s">
@@ -21052,7 +21052,7 @@
       <c r="T464" s="8"/>
       <c r="U464" s="8"/>
       <c r="V464" s="45" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="465" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21186,7 +21186,7 @@
       <c r="T468" s="8"/>
       <c r="U468" s="8"/>
       <c r="V468" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="469" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21259,7 +21259,7 @@
     </row>
     <row r="471" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A471" s="8" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D471" s="24"/>
       <c r="H471" s="50" t="s">
@@ -21394,7 +21394,7 @@
         <v>76</v>
       </c>
       <c r="T474" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="U474" s="8"/>
       <c r="V474" s="45"/>
@@ -21528,7 +21528,7 @@
       <c r="T478" s="8"/>
       <c r="U478" s="8"/>
       <c r="V478" s="45" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="479" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21567,7 +21567,7 @@
       <c r="T479" s="8"/>
       <c r="U479" s="8"/>
       <c r="V479" s="45" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="480" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21940,7 +21940,7 @@
       <c r="T490" s="8"/>
       <c r="U490" s="8"/>
       <c r="V490" s="45" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="491" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22070,7 +22070,7 @@
         <v>76</v>
       </c>
       <c r="T494" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="U494" s="8"/>
       <c r="V494" s="45"/>
@@ -22172,7 +22172,7 @@
       <c r="T497" s="8"/>
       <c r="U497" s="8"/>
       <c r="V497" s="45" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="498" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22368,7 +22368,7 @@
       <c r="T503" s="8"/>
       <c r="U503" s="8"/>
       <c r="V503" s="45" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="504" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22436,7 +22436,7 @@
       <c r="T505" s="8"/>
       <c r="U505" s="8"/>
       <c r="V505" s="45" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="506" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22810,7 +22810,7 @@
       <c r="T515" s="8"/>
       <c r="U515" s="8"/>
       <c r="V515" s="45" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="516" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23127,7 +23127,7 @@
       <c r="T524" s="8"/>
       <c r="U524" s="8"/>
       <c r="V524" s="45" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="525" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23325,7 +23325,7 @@
       <c r="T530" s="8"/>
       <c r="U530" s="8"/>
       <c r="V530" s="45" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="531" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23361,7 +23361,7 @@
       <c r="T531" s="8"/>
       <c r="U531" s="8"/>
       <c r="V531" s="45" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="532" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23397,7 +23397,7 @@
       <c r="T532" s="8"/>
       <c r="U532" s="8"/>
       <c r="V532" s="45" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="533" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23657,7 +23657,7 @@
       <c r="T540" s="8"/>
       <c r="U540" s="8"/>
       <c r="V540" s="45" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="541" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23693,7 +23693,7 @@
       <c r="T541" s="8"/>
       <c r="U541" s="8"/>
       <c r="V541" s="45" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="542" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23764,7 +23764,7 @@
       <c r="T543" s="8"/>
       <c r="U543" s="8"/>
       <c r="V543" s="45" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="544" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23838,7 +23838,7 @@
       <c r="T545" s="8"/>
       <c r="U545" s="8"/>
       <c r="V545" s="45" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="546" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24017,7 +24017,7 @@
       <c r="T550" s="8"/>
       <c r="U550" s="8"/>
       <c r="V550" s="45" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="551" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24252,7 +24252,7 @@
       <c r="T557" s="8"/>
       <c r="U557" s="8"/>
       <c r="V557" s="45" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="558" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24287,7 +24287,7 @@
       <c r="T558" s="8"/>
       <c r="U558" s="8"/>
       <c r="V558" s="45" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="559" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24485,7 +24485,7 @@
       <c r="T564" s="8"/>
       <c r="U564" s="8"/>
       <c r="V564" s="45" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="565" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24553,7 +24553,7 @@
       <c r="T566" s="8"/>
       <c r="U566" s="8"/>
       <c r="V566" s="45" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="567" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24621,7 +24621,7 @@
       <c r="T568" s="8"/>
       <c r="U568" s="8"/>
       <c r="V568" s="45" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="569" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24657,7 +24657,7 @@
       <c r="T569" s="8"/>
       <c r="U569" s="8"/>
       <c r="V569" s="45" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="570" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24885,7 +24885,7 @@
       <c r="T576" s="8"/>
       <c r="U576" s="8"/>
       <c r="V576" s="45" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="577" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24953,7 +24953,7 @@
       <c r="T578" s="8"/>
       <c r="U578" s="8"/>
       <c r="V578" s="45" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="579" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24989,7 +24989,7 @@
       <c r="T579" s="8"/>
       <c r="U579" s="8"/>
       <c r="V579" s="45" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="580" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25153,7 +25153,7 @@
       <c r="T584" s="8"/>
       <c r="U584" s="8"/>
       <c r="V584" s="45" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="585" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25221,7 +25221,7 @@
       <c r="T586" s="8"/>
       <c r="U586" s="8"/>
       <c r="V586" s="45" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="587" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25419,7 +25419,7 @@
       <c r="T592" s="8"/>
       <c r="U592" s="8"/>
       <c r="V592" s="45" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="593" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25455,7 +25455,7 @@
       <c r="T593" s="8"/>
       <c r="U593" s="8"/>
       <c r="V593" s="45" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="594" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25523,7 +25523,7 @@
       <c r="T595" s="8"/>
       <c r="U595" s="8"/>
       <c r="V595" s="45" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="596" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25591,7 +25591,7 @@
       <c r="T597" s="8"/>
       <c r="U597" s="8"/>
       <c r="V597" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="598" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25755,7 +25755,7 @@
       <c r="T602" s="8"/>
       <c r="U602" s="8"/>
       <c r="V602" s="45" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="603" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25791,7 +25791,7 @@
       <c r="T603" s="8"/>
       <c r="U603" s="8"/>
       <c r="V603" s="45" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="604" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25986,7 +25986,7 @@
       <c r="T609" s="8"/>
       <c r="U609" s="8"/>
       <c r="V609" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="610" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26011,7 +26011,7 @@
         <v>53</v>
       </c>
       <c r="N610" s="46" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="O610" s="7"/>
       <c r="P610" s="8"/>
@@ -26416,7 +26416,7 @@
       <c r="T622" s="8"/>
       <c r="U622" s="8"/>
       <c r="V622" s="45" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="623" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26452,7 +26452,7 @@
       <c r="T623" s="8"/>
       <c r="U623" s="8"/>
       <c r="V623" s="45" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="624" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26520,7 +26520,7 @@
       <c r="T625" s="8"/>
       <c r="U625" s="8"/>
       <c r="V625" s="45" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="626" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26588,7 +26588,7 @@
       <c r="T627" s="8"/>
       <c r="U627" s="8"/>
       <c r="V627" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="628" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26722,7 +26722,7 @@
       <c r="T631" s="20"/>
       <c r="U631" s="20"/>
       <c r="V631" s="45" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="632" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26758,7 +26758,7 @@
       <c r="T632" s="8"/>
       <c r="U632" s="8"/>
       <c r="V632" s="45" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="633" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26826,7 +26826,7 @@
       <c r="T634" s="8"/>
       <c r="U634" s="8"/>
       <c r="V634" s="45" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="635" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26926,7 +26926,7 @@
       <c r="T637" s="8"/>
       <c r="U637" s="8"/>
       <c r="V637" s="45" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="638" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26992,7 +26992,7 @@
       <c r="T639" s="8"/>
       <c r="U639" s="8"/>
       <c r="V639" s="45" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="640" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27028,7 +27028,7 @@
       <c r="T640" s="8"/>
       <c r="U640" s="8"/>
       <c r="V640" s="45" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="641" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27356,7 +27356,7 @@
       <c r="T650" s="8"/>
       <c r="U650" s="8"/>
       <c r="V650" s="45" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="651" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27714,7 +27714,7 @@
       <c r="T661" s="8"/>
       <c r="U661" s="8"/>
       <c r="V661" s="45" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="662" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27922,7 +27922,7 @@
     </row>
     <row r="668" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A668" s="61" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H668" s="50" t="s">
         <v>89</v>
@@ -28053,7 +28053,7 @@
       <c r="T671" s="8"/>
       <c r="U671" s="8"/>
       <c r="V671" s="45" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="672" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -28181,7 +28181,7 @@
       <c r="T675" s="8"/>
       <c r="U675" s="8"/>
       <c r="V675" s="45" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="676" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -28906,7 +28906,7 @@
     </row>
     <row r="699" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A699" s="62" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="I699" s="48" t="s">
         <v>35</v>
@@ -29657,7 +29657,7 @@
       <c r="T722" s="8"/>
       <c r="U722" s="8"/>
       <c r="V722" s="45" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="723" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30041,7 +30041,7 @@
       <c r="T734" s="8"/>
       <c r="U734" s="8"/>
       <c r="V734" s="45" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="735" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30172,7 +30172,7 @@
       <c r="T738" s="8"/>
       <c r="U738" s="8"/>
       <c r="V738" s="45" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="739" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30300,7 +30300,7 @@
       <c r="T742" s="8"/>
       <c r="U742" s="8"/>
       <c r="V742" s="45" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="743" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30428,7 +30428,7 @@
       <c r="T746" s="8"/>
       <c r="U746" s="8"/>
       <c r="V746" s="45" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="747" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30649,7 +30649,7 @@
       <c r="T753" s="8"/>
       <c r="U753" s="8"/>
       <c r="V753" s="45" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="754" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30777,7 +30777,7 @@
       <c r="T757" s="8"/>
       <c r="U757" s="8"/>
       <c r="V757" s="45" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="758" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31378,7 +31378,7 @@
       <c r="T776" s="8"/>
       <c r="U776" s="8"/>
       <c r="V776" s="45" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="777" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31413,7 +31413,7 @@
       <c r="T777" s="8"/>
       <c r="U777" s="8"/>
       <c r="V777" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="778" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31510,7 +31510,7 @@
       <c r="T780" s="8"/>
       <c r="U780" s="8"/>
       <c r="V780" s="45" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="781" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31548,7 +31548,7 @@
       <c r="T781" s="8"/>
       <c r="U781" s="8"/>
       <c r="V781" s="45" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="782" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31847,7 +31847,7 @@
       <c r="S790" s="8"/>
       <c r="T790" s="8"/>
       <c r="V790" s="45" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="791" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31913,7 +31913,7 @@
       <c r="T792" s="8"/>
       <c r="U792" s="8"/>
       <c r="V792" s="45" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="793" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32136,7 +32136,7 @@
       <c r="T799" s="8"/>
       <c r="U799" s="8"/>
       <c r="V799" s="45" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="800" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32208,7 +32208,7 @@
       <c r="T801" s="8"/>
       <c r="U801" s="8"/>
       <c r="V801" s="45" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="802" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32276,7 +32276,7 @@
       <c r="T803" s="8"/>
       <c r="U803" s="8"/>
       <c r="V803" s="45" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="804" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32342,7 +32342,7 @@
       <c r="T805" s="8"/>
       <c r="U805" s="8"/>
       <c r="V805" s="45" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="806" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32470,7 +32470,7 @@
       <c r="T809" s="8"/>
       <c r="U809" s="8"/>
       <c r="V809" s="45" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="810" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32505,7 +32505,7 @@
       <c r="T810" s="8"/>
       <c r="U810" s="8"/>
       <c r="V810" s="45" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="811" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32664,7 +32664,7 @@
       <c r="T815" s="8"/>
       <c r="U815" s="8"/>
       <c r="V815" s="45" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="816" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32728,7 +32728,7 @@
       <c r="T817" s="8"/>
       <c r="U817" s="8"/>
       <c r="V817" s="45" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="818" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32825,7 +32825,7 @@
       <c r="T820" s="8"/>
       <c r="U820" s="8"/>
       <c r="V820" s="45" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="821" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32922,7 +32922,7 @@
       <c r="T823" s="8"/>
       <c r="U823" s="8"/>
       <c r="V823" s="45" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="824" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33455,7 +33455,7 @@
       <c r="T840" s="8"/>
       <c r="U840" s="8"/>
       <c r="V840" s="45" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="841" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33648,7 +33648,7 @@
       <c r="T846" s="8"/>
       <c r="U846" s="8"/>
       <c r="V846" s="45" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="847" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34090,7 +34090,7 @@
       <c r="T860" s="8"/>
       <c r="U860" s="8"/>
       <c r="V860" s="45" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="861" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34949,7 +34949,7 @@
       <c r="T887" s="8"/>
       <c r="U887" s="8"/>
       <c r="V887" s="45" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="888" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35356,7 +35356,7 @@
       <c r="T900" s="8"/>
       <c r="U900" s="8"/>
       <c r="V900" s="45" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="901" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35873,7 +35873,7 @@
     </row>
     <row r="917" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A917" s="63" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="H917" s="50" t="s">
         <v>92</v>
@@ -35907,7 +35907,7 @@
         <v>76</v>
       </c>
       <c r="T917" s="8" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="U917" s="8"/>
       <c r="V917" s="45"/>
@@ -36046,7 +36046,7 @@
       <c r="T921" s="8"/>
       <c r="U921" s="8"/>
       <c r="V921" s="45" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="922" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36127,7 +36127,7 @@
       <c r="T923" s="8"/>
       <c r="U923" s="8"/>
       <c r="V923" s="45" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="924" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36499,7 +36499,7 @@
       <c r="T934" s="8"/>
       <c r="U934" s="8"/>
       <c r="V934" s="45" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="935" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36693,7 +36693,7 @@
       <c r="T940" s="8"/>
       <c r="U940" s="8"/>
       <c r="V940" s="45" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="941" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36759,7 +36759,7 @@
         <v>81</v>
       </c>
       <c r="T942" s="8" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="U942" s="8"/>
       <c r="V942" s="45"/>
@@ -36858,7 +36858,7 @@
       <c r="T945" s="8"/>
       <c r="U945" s="8"/>
       <c r="V945" s="45" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="946" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36955,7 +36955,7 @@
       <c r="T948" s="8"/>
       <c r="U948" s="8"/>
       <c r="V948" s="45" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="949" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37021,7 +37021,7 @@
       <c r="T950" s="8"/>
       <c r="U950" s="8"/>
       <c r="V950" s="45" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="951" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37056,7 +37056,7 @@
       <c r="T951" s="8"/>
       <c r="U951" s="8"/>
       <c r="V951" s="45" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="952" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38020,7 +38020,7 @@
       <c r="T982" s="8"/>
       <c r="U982" s="8"/>
       <c r="V982" s="45" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="983" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38056,7 +38056,7 @@
       <c r="T983" s="8"/>
       <c r="U983" s="8"/>
       <c r="V983" s="45" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="984" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38374,7 +38374,7 @@
       <c r="T993" s="8"/>
       <c r="U993" s="8"/>
       <c r="V993" s="45" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="994" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38440,7 +38440,7 @@
       <c r="T995" s="8"/>
       <c r="U995" s="8"/>
       <c r="V995" s="45" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="996" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38888,7 +38888,7 @@
       <c r="T1009" s="8"/>
       <c r="U1009" s="8"/>
       <c r="V1009" s="45" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="1010" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39278,7 +39278,7 @@
       <c r="T1021" s="8"/>
       <c r="U1021" s="8"/>
       <c r="V1021" s="45" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="1022" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39415,7 +39415,7 @@
       <c r="T1025" s="8"/>
       <c r="U1025" s="8"/>
       <c r="V1025" s="45" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="1026" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39547,7 +39547,7 @@
       <c r="T1029" s="8"/>
       <c r="U1029" s="8"/>
       <c r="V1029" s="45" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="1030" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39706,7 +39706,7 @@
       <c r="T1034" s="8"/>
       <c r="U1034" s="8"/>
       <c r="V1034" s="45" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="1035" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39899,7 +39899,7 @@
       <c r="T1040" s="8"/>
       <c r="U1040" s="8"/>
       <c r="V1040" s="45" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="1041" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40216,7 +40216,7 @@
       <c r="T1050" s="8"/>
       <c r="U1050" s="8"/>
       <c r="V1050" s="45" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="1051" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40470,7 +40470,7 @@
       <c r="T1058" s="8"/>
       <c r="U1058" s="8"/>
       <c r="V1058" s="45" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="1059" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40815,7 +40815,7 @@
       <c r="T1069" s="8"/>
       <c r="U1069" s="8"/>
       <c r="V1069" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1070" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40850,7 +40850,7 @@
       <c r="T1070" s="8"/>
       <c r="U1070" s="8"/>
       <c r="V1070" s="45" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="1071" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41042,7 +41042,7 @@
       <c r="T1076" s="8"/>
       <c r="U1076" s="8"/>
       <c r="V1076" s="45" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="1077" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41108,7 +41108,7 @@
       <c r="T1078" s="8"/>
       <c r="U1078" s="8"/>
       <c r="V1078" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1079" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41144,7 +41144,7 @@
       <c r="T1079" s="8"/>
       <c r="U1079" s="8"/>
       <c r="V1079" s="45" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="1080" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41354,7 +41354,7 @@
       <c r="T1085" s="8"/>
       <c r="U1085" s="8"/>
       <c r="V1085" s="45" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="1086" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41456,7 +41456,7 @@
       <c r="T1088" s="8"/>
       <c r="U1088" s="8"/>
       <c r="V1088" s="45" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="1089" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41590,7 +41590,7 @@
       <c r="T1092" s="8"/>
       <c r="U1092" s="8"/>
       <c r="V1092" s="45" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="1093" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41623,7 +41623,7 @@
       <c r="T1093" s="8"/>
       <c r="U1093" s="8"/>
       <c r="V1093" s="45" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="1094" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41752,7 +41752,7 @@
       <c r="T1097" s="8"/>
       <c r="U1097" s="8"/>
       <c r="V1097" s="45" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="1098" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41916,7 +41916,7 @@
       <c r="T1102" s="8"/>
       <c r="U1102" s="8"/>
       <c r="V1102" s="45" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="1103" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41952,7 +41952,7 @@
       <c r="T1103" s="8"/>
       <c r="U1103" s="8"/>
       <c r="V1103" s="45" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="1104" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42115,7 +42115,7 @@
       <c r="T1108" s="8"/>
       <c r="U1108" s="8"/>
       <c r="V1108" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1109" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42150,7 +42150,7 @@
       <c r="T1109" s="8"/>
       <c r="U1109" s="8"/>
       <c r="V1109" s="45" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="1110" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42342,7 +42342,7 @@
       <c r="T1115" s="8"/>
       <c r="U1115" s="8"/>
       <c r="V1115" s="45" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="1116" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42408,7 +42408,7 @@
       <c r="T1117" s="8"/>
       <c r="U1117" s="8"/>
       <c r="V1117" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1118" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42443,7 +42443,7 @@
       <c r="T1118" s="8"/>
       <c r="U1118" s="8"/>
       <c r="V1118" s="45" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="1119" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42884,7 +42884,7 @@
       <c r="T1132" s="8"/>
       <c r="U1132" s="8"/>
       <c r="V1132" s="45" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="1133" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43141,7 +43141,7 @@
         <v>81</v>
       </c>
       <c r="T1140" s="8" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="U1140" s="8"/>
       <c r="V1140" s="45"/>
@@ -43493,7 +43493,7 @@
       <c r="T1151" s="8"/>
       <c r="U1151" s="8"/>
       <c r="V1151" s="45" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="1152" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43562,7 +43562,7 @@
       <c r="T1153" s="8"/>
       <c r="U1153" s="8"/>
       <c r="V1153" s="45" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="1154" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43666,7 +43666,7 @@
         <v>81</v>
       </c>
       <c r="T1156" s="8" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="V1156" s="45"/>
     </row>
@@ -43954,7 +43954,7 @@
       <c r="S1165" s="8"/>
       <c r="T1165" s="8"/>
       <c r="V1165" s="45" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="1166" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44115,7 +44115,7 @@
       <c r="T1170" s="8"/>
       <c r="U1170" s="8"/>
       <c r="V1170" s="45" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="1171" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44150,7 +44150,7 @@
       <c r="T1171" s="8"/>
       <c r="U1171" s="8"/>
       <c r="V1171" s="45" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="1172" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44185,7 +44185,7 @@
       <c r="T1172" s="8"/>
       <c r="U1172" s="8"/>
       <c r="V1172" s="45" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="1173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44282,7 +44282,7 @@
       <c r="T1175" s="8"/>
       <c r="U1175" s="8"/>
       <c r="V1175" s="45" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="1176" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44348,7 +44348,7 @@
       <c r="T1177" s="8"/>
       <c r="U1177" s="8"/>
       <c r="V1177" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1178" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44383,7 +44383,7 @@
       <c r="T1178" s="8"/>
       <c r="U1178" s="8"/>
       <c r="V1178" s="45" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="1179" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44480,7 +44480,7 @@
       <c r="T1181" s="8"/>
       <c r="U1181" s="8"/>
       <c r="V1181" s="45" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="1182" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44577,7 +44577,7 @@
       <c r="T1184" s="8"/>
       <c r="U1184" s="8"/>
       <c r="V1184" s="45" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="1185" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44612,7 +44612,7 @@
       <c r="T1185" s="8"/>
       <c r="U1185" s="8"/>
       <c r="V1185" s="45" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="1186" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44709,7 +44709,7 @@
       <c r="T1188" s="8"/>
       <c r="U1188" s="8"/>
       <c r="V1188" s="45" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="1189" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44806,7 +44806,7 @@
       <c r="T1191" s="8"/>
       <c r="U1191" s="8"/>
       <c r="V1191" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1192" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45154,7 +45154,7 @@
       <c r="T1202" s="8"/>
       <c r="U1202" s="8"/>
       <c r="V1202" s="45" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="1203" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45220,7 +45220,7 @@
       <c r="T1204" s="8"/>
       <c r="U1204" s="8"/>
       <c r="V1204" s="45" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="1205" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45410,7 +45410,7 @@
       <c r="T1210" s="8"/>
       <c r="U1210" s="8"/>
       <c r="V1210" s="45" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="1211" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45445,7 +45445,7 @@
       <c r="T1211" s="8"/>
       <c r="U1211" s="8"/>
       <c r="V1211" s="45" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="1212" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45668,7 +45668,7 @@
       <c r="T1218" s="8"/>
       <c r="U1218" s="8"/>
       <c r="V1218" s="45" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="1219" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45734,7 +45734,7 @@
       <c r="T1220" s="8"/>
       <c r="U1220" s="8"/>
       <c r="V1220" s="45" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="1221" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45800,7 +45800,7 @@
       <c r="T1222" s="8"/>
       <c r="U1222" s="8"/>
       <c r="V1222" s="45" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="1223" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46358,7 +46358,7 @@
       <c r="T1239" s="8"/>
       <c r="U1239" s="8"/>
       <c r="V1239" s="45" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="1240" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46982,7 +46982,7 @@
       <c r="T1259" s="8"/>
       <c r="U1259" s="8"/>
       <c r="V1259" s="45" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="1260" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47048,7 +47048,7 @@
       <c r="T1261" s="8"/>
       <c r="U1261" s="8"/>
       <c r="V1261" s="45" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="1262" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47069,7 +47069,7 @@
         <v>1</v>
       </c>
       <c r="N1262" s="46" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O1262" s="8" t="s">
         <v>62</v>
@@ -47081,7 +47081,7 @@
       <c r="T1262" s="8"/>
       <c r="U1262" s="8"/>
       <c r="V1262" s="46" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="1263" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47209,7 +47209,7 @@
       <c r="T1266" s="8"/>
       <c r="U1266" s="8"/>
       <c r="V1266" s="45" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1267" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47276,7 +47276,7 @@
       <c r="T1268" s="8"/>
       <c r="U1268" s="8"/>
       <c r="V1268" s="45" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="1269" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47377,7 +47377,7 @@
       <c r="T1271" s="8"/>
       <c r="U1271" s="8"/>
       <c r="V1271" s="45" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="1272" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47474,7 +47474,7 @@
       <c r="T1274" s="8"/>
       <c r="U1274" s="8"/>
       <c r="V1274" s="45" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="1275" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47509,7 +47509,7 @@
       <c r="T1275" s="8"/>
       <c r="U1275" s="8"/>
       <c r="V1275" s="45" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="1276" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47608,7 +47608,7 @@
       <c r="T1278" s="8"/>
       <c r="U1278" s="8"/>
       <c r="V1278" s="45" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1279" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47643,7 +47643,7 @@
       <c r="T1279" s="8"/>
       <c r="U1279" s="8"/>
       <c r="V1279" s="45" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="1280" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47775,7 +47775,7 @@
       <c r="T1283" s="8"/>
       <c r="U1283" s="8"/>
       <c r="V1283" s="45" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="1284" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47922,7 +47922,7 @@
         <v>27</v>
       </c>
       <c r="N1288" s="46" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O1288" s="8" t="s">
         <v>62</v>
@@ -47934,7 +47934,7 @@
       <c r="T1288" s="8"/>
       <c r="U1288" s="8"/>
       <c r="V1288" s="46" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="1289" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47969,7 +47969,7 @@
       <c r="T1289" s="8"/>
       <c r="U1289" s="8"/>
       <c r="V1289" s="45" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1290" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48035,7 +48035,7 @@
       <c r="T1291" s="8"/>
       <c r="U1291" s="8"/>
       <c r="V1291" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1292" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48165,7 +48165,7 @@
       <c r="T1295" s="8"/>
       <c r="U1295" s="8"/>
       <c r="V1295" s="45" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="1296" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48200,7 +48200,7 @@
       <c r="T1296" s="8"/>
       <c r="U1296" s="8"/>
       <c r="V1296" s="45" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1297" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48297,7 +48297,7 @@
       <c r="T1299" s="8"/>
       <c r="U1299" s="8"/>
       <c r="V1299" s="45" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="1300" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48332,7 +48332,7 @@
       <c r="T1300" s="8"/>
       <c r="U1300" s="8"/>
       <c r="V1300" s="45" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="1301" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48398,7 +48398,7 @@
       <c r="T1302" s="8"/>
       <c r="U1302" s="8"/>
       <c r="V1302" s="45" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="1303" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48433,7 +48433,7 @@
       <c r="T1303" s="8"/>
       <c r="U1303" s="8"/>
       <c r="V1303" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1304" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48637,7 +48637,7 @@
       <c r="T1309" s="8"/>
       <c r="U1309" s="8"/>
       <c r="V1309" s="45" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="1310" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48707,7 +48707,7 @@
       <c r="T1311" s="8"/>
       <c r="U1311" s="8"/>
       <c r="V1311" s="45" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1312" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48838,7 +48838,7 @@
       <c r="T1315" s="8"/>
       <c r="U1315" s="8"/>
       <c r="V1315" s="45" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1316" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49084,7 +49084,7 @@
       <c r="T1322" s="8"/>
       <c r="U1322" s="8"/>
       <c r="V1322" s="45" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1323" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49317,7 +49317,7 @@
       <c r="T1329" s="8"/>
       <c r="U1329" s="8"/>
       <c r="V1329" s="45" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1330" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49484,7 +49484,7 @@
       <c r="S1334" s="8"/>
       <c r="T1334" s="8"/>
       <c r="V1334" s="45" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="1335" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49552,7 +49552,7 @@
       <c r="T1336" s="8"/>
       <c r="U1336" s="8"/>
       <c r="V1336" s="45" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="1337" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49620,7 +49620,7 @@
       <c r="T1338" s="8"/>
       <c r="U1338" s="8"/>
       <c r="V1338" s="45" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="1339" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50040,7 +50040,7 @@
       <c r="T1351" s="8"/>
       <c r="U1351" s="8"/>
       <c r="V1351" s="45" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="1352" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50204,7 +50204,7 @@
       <c r="T1356" s="8"/>
       <c r="U1356" s="8"/>
       <c r="V1356" s="45" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1357" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50243,7 +50243,7 @@
       <c r="T1357" s="8"/>
       <c r="U1357" s="8"/>
       <c r="V1357" s="45" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="1358" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50387,7 +50387,7 @@
       <c r="T1361" s="8"/>
       <c r="U1361" s="8"/>
       <c r="V1361" s="45" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="1362" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50519,7 +50519,7 @@
       <c r="T1365" s="8"/>
       <c r="U1365" s="8"/>
       <c r="V1365" s="45" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1366" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50786,7 +50786,7 @@
       <c r="T1373" s="8"/>
       <c r="U1373" s="8"/>
       <c r="V1373" s="45" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="1374" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50983,7 +50983,7 @@
       <c r="T1379" s="8"/>
       <c r="U1379" s="8"/>
       <c r="V1379" s="45" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51086,7 +51086,7 @@
       <c r="T1382" s="8"/>
       <c r="U1382" s="8"/>
       <c r="V1382" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1383" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51227,7 +51227,7 @@
       <c r="T1386" s="8"/>
       <c r="U1386" s="8"/>
       <c r="V1386" s="45" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1387" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51583,7 +51583,7 @@
       <c r="T1397" s="8"/>
       <c r="U1397" s="8"/>
       <c r="V1397" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1398" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51688,7 +51688,7 @@
       <c r="T1400" s="8"/>
       <c r="U1400" s="8"/>
       <c r="V1400" s="45" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1401" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52017,7 +52017,7 @@
         <v>149</v>
       </c>
       <c r="N1410" s="46" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="O1410" s="8" t="s">
         <v>62</v>
@@ -52029,7 +52029,7 @@
       <c r="T1410" s="8"/>
       <c r="U1410" s="8"/>
       <c r="V1410" s="45" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1411" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52128,7 +52128,7 @@
       <c r="T1413" s="8"/>
       <c r="U1413" s="8"/>
       <c r="V1413" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1414" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52228,7 +52228,7 @@
       <c r="T1416" s="8"/>
       <c r="U1416" s="8"/>
       <c r="V1416" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1417" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52366,7 +52366,7 @@
     </row>
     <row r="1421" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1421" s="66" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B1421" s="67"/>
       <c r="C1421" s="68"/>
@@ -52394,7 +52394,7 @@
         <v>160</v>
       </c>
       <c r="N1421" s="64" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1421" s="7"/>
       <c r="P1421" s="8"/>
@@ -52578,7 +52578,7 @@
       <c r="T1426" s="8"/>
       <c r="U1426" s="8"/>
       <c r="V1426" s="45" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1427" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52614,7 +52614,7 @@
       <c r="T1427" s="8"/>
       <c r="U1427" s="8"/>
       <c r="V1427" s="45" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1428" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52714,7 +52714,7 @@
       <c r="T1430" s="8"/>
       <c r="U1430" s="8"/>
       <c r="V1430" s="45" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1431" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52750,7 +52750,7 @@
       <c r="T1431" s="8"/>
       <c r="U1431" s="8"/>
       <c r="V1431" s="45" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1432" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53106,7 +53106,7 @@
       <c r="T1442" s="8"/>
       <c r="U1442" s="8"/>
       <c r="V1442" s="45" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1443" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53799,7 +53799,7 @@
       <c r="T1463" s="8"/>
       <c r="U1463" s="8"/>
       <c r="V1463" s="45" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="1464" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53999,7 +53999,7 @@
       <c r="T1469" s="8"/>
       <c r="U1469" s="8"/>
       <c r="V1469" s="45" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1470" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54265,7 +54265,7 @@
       <c r="T1477" s="8"/>
       <c r="U1477" s="8"/>
       <c r="V1477" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1478" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54302,7 +54302,7 @@
       <c r="T1478" s="8"/>
       <c r="U1478" s="8"/>
       <c r="V1478" s="45" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="1479" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54502,7 +54502,7 @@
       <c r="S1484" s="8"/>
       <c r="T1484" s="8"/>
       <c r="V1484" s="45" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="1485" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54570,7 +54570,7 @@
       <c r="T1486" s="8"/>
       <c r="U1486" s="8"/>
       <c r="V1486" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1487" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54606,7 +54606,7 @@
       <c r="T1487" s="8"/>
       <c r="U1487" s="8"/>
       <c r="V1487" s="45" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="1488" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54706,7 +54706,7 @@
       <c r="T1490" s="8"/>
       <c r="U1490" s="8"/>
       <c r="V1490" s="45" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="1491" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54774,7 +54774,7 @@
       <c r="T1492" s="8"/>
       <c r="U1492" s="8"/>
       <c r="V1492" s="45" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1493" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54874,7 +54874,7 @@
       <c r="T1495" s="8"/>
       <c r="U1495" s="8"/>
       <c r="V1495" s="45" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1496" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55071,7 +55071,7 @@
       <c r="T1501" s="8"/>
       <c r="U1501" s="8"/>
       <c r="V1501" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1502" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55108,7 +55108,7 @@
       <c r="T1502" s="8"/>
       <c r="U1502" s="8"/>
       <c r="V1502" s="45" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1503" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55177,7 +55177,7 @@
       <c r="T1504" s="8"/>
       <c r="U1504" s="8"/>
       <c r="V1504" s="45" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1505" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55280,7 +55280,7 @@
       <c r="T1507" s="8"/>
       <c r="U1507" s="8"/>
       <c r="V1507" s="45" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1508" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55354,7 +55354,7 @@
       <c r="T1509" s="8"/>
       <c r="U1509" s="8"/>
       <c r="V1509" s="45" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1510" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55534,7 +55534,7 @@
       <c r="T1514" s="8"/>
       <c r="U1514" s="8"/>
       <c r="V1514" s="45" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1515" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55636,7 +55636,7 @@
       <c r="T1517" s="8"/>
       <c r="U1517" s="8"/>
       <c r="V1517" s="45" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1518" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55864,7 +55864,7 @@
       <c r="T1524" s="8"/>
       <c r="U1524" s="8"/>
       <c r="V1524" s="45" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1525" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55966,7 +55966,7 @@
       <c r="T1527" s="8"/>
       <c r="U1527" s="8"/>
       <c r="V1527" s="45" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="1528" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56097,7 +56097,7 @@
       <c r="T1531" s="8"/>
       <c r="U1531" s="8"/>
       <c r="V1531" s="45" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1532" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56132,7 +56132,7 @@
       <c r="T1532" s="8"/>
       <c r="U1532" s="8"/>
       <c r="V1532" s="45" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="1533" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56170,7 +56170,7 @@
       <c r="T1533" s="8"/>
       <c r="U1533" s="8"/>
       <c r="V1533" s="45" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="1534" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56757,7 +56757,7 @@
       <c r="T1550" s="8"/>
       <c r="U1550" s="8"/>
       <c r="V1550" s="45" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1551" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57316,7 +57316,7 @@
       <c r="T1567" s="8"/>
       <c r="U1567" s="8"/>
       <c r="V1567" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1568" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57384,7 +57384,7 @@
       <c r="T1569" s="8"/>
       <c r="U1569" s="8"/>
       <c r="V1569" s="45" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1570" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57541,7 +57541,7 @@
       <c r="T1574" s="8"/>
       <c r="U1574" s="8"/>
       <c r="V1574" s="45" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1575" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57671,7 +57671,7 @@
       <c r="T1578" s="8"/>
       <c r="U1578" s="8"/>
       <c r="V1578" s="45" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1579" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57854,7 +57854,7 @@
         <v>62</v>
       </c>
       <c r="V1585" s="45" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1586" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58294,7 +58294,7 @@
         <v>62</v>
       </c>
       <c r="V1603" s="45" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1604" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58850,7 +58850,7 @@
         <v>62</v>
       </c>
       <c r="V1626" s="45" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1627" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58903,7 +58903,7 @@
         <v>62</v>
       </c>
       <c r="V1628" s="45" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="1629" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59220,7 +59220,7 @@
         <v>62</v>
       </c>
       <c r="V1641" s="45" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1642" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59273,7 +59273,7 @@
         <v>64</v>
       </c>
       <c r="V1643" s="45" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1644" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59446,7 +59446,7 @@
         <v>62</v>
       </c>
       <c r="V1650" s="45" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1651" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59499,7 +59499,7 @@
         <v>62</v>
       </c>
       <c r="V1652" s="45" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1653" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59624,7 +59624,7 @@
         <v>66</v>
       </c>
       <c r="V1657" s="45" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1658" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59701,7 +59701,7 @@
         <v>64</v>
       </c>
       <c r="V1660" s="45" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1661" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59730,7 +59730,7 @@
         <v>62</v>
       </c>
       <c r="V1661" s="45" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1662" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59783,7 +59783,7 @@
         <v>62</v>
       </c>
       <c r="V1663" s="45" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1664" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59812,7 +59812,7 @@
         <v>62</v>
       </c>
       <c r="V1664" s="45" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1665" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59865,7 +59865,7 @@
         <v>62</v>
       </c>
       <c r="V1666" s="45" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1667" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59894,7 +59894,7 @@
         <v>62</v>
       </c>
       <c r="V1667" s="45" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1668" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59947,7 +59947,7 @@
         <v>62</v>
       </c>
       <c r="V1669" s="45" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1670" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60050,7 +60050,7 @@
         <v>62</v>
       </c>
       <c r="V1673" s="45" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1674" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60079,7 +60079,7 @@
         <v>62</v>
       </c>
       <c r="V1674" s="45" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1675" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60132,7 +60132,7 @@
         <v>62</v>
       </c>
       <c r="V1676" s="45" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1677" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60260,7 +60260,7 @@
         <v>62</v>
       </c>
       <c r="V1681" s="45" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1682" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60316,7 +60316,7 @@
         <v>62</v>
       </c>
       <c r="V1683" s="45" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1684" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60453,7 +60453,7 @@
         <v>62</v>
       </c>
       <c r="V1688" s="45" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1689" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60578,7 +60578,7 @@
         <v>62</v>
       </c>
       <c r="V1693" s="45" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="1694" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60607,7 +60607,7 @@
         <v>76</v>
       </c>
       <c r="T1694" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="V1694" s="45"/>
     </row>
@@ -60757,7 +60757,7 @@
         <v>62</v>
       </c>
       <c r="V1700" s="45" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1701" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60882,7 +60882,7 @@
         <v>62</v>
       </c>
       <c r="V1705" s="45" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1706" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60911,7 +60911,7 @@
         <v>62</v>
       </c>
       <c r="V1706" s="45" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1707" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60964,7 +60964,7 @@
         <v>62</v>
       </c>
       <c r="V1708" s="45" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1709" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61089,7 +61089,7 @@
         <v>62</v>
       </c>
       <c r="V1713" s="45" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1714" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61166,7 +61166,7 @@
         <v>62</v>
       </c>
       <c r="V1716" s="45" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1717" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61219,7 +61219,7 @@
         <v>62</v>
       </c>
       <c r="V1718" s="45" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1719" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61457,7 +61457,7 @@
         <v>62</v>
       </c>
       <c r="V1727" s="45" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1728" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61930,7 +61930,7 @@
         <v>62</v>
       </c>
       <c r="V1746" s="45" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1747" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61959,7 +61959,7 @@
         <v>62</v>
       </c>
       <c r="V1747" s="45" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1748" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62084,7 +62084,7 @@
         <v>62</v>
       </c>
       <c r="V1752" s="45" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="1753" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62212,7 +62212,7 @@
         <v>62</v>
       </c>
       <c r="V1757" s="45" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="1758" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62340,7 +62340,7 @@
         <v>62</v>
       </c>
       <c r="V1762" s="45" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1763" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62393,7 +62393,7 @@
         <v>62</v>
       </c>
       <c r="V1764" s="45" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1765" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62521,13 +62521,13 @@
         <v>63</v>
       </c>
       <c r="S1769" s="8" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="T1769" s="8" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="V1769" s="46" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1770" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62629,7 +62629,7 @@
         <v>62</v>
       </c>
       <c r="V1773" s="45" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1774" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62733,7 +62733,7 @@
         <v>62</v>
       </c>
       <c r="V1777" s="45" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1778" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62762,7 +62762,7 @@
         <v>62</v>
       </c>
       <c r="V1778" s="45" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1779" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62791,7 +62791,7 @@
         <v>62</v>
       </c>
       <c r="V1779" s="45" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1780" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62844,7 +62844,7 @@
         <v>62</v>
       </c>
       <c r="V1781" s="45" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1782" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62873,7 +62873,7 @@
         <v>62</v>
       </c>
       <c r="V1782" s="45" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1783" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62902,7 +62902,7 @@
         <v>62</v>
       </c>
       <c r="V1783" s="45" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1784" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62955,7 +62955,7 @@
         <v>62</v>
       </c>
       <c r="V1785" s="45" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1786" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63008,7 +63008,7 @@
         <v>62</v>
       </c>
       <c r="V1787" s="45" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="1788" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63205,7 +63205,7 @@
         <v>62</v>
       </c>
       <c r="V1795" s="45" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1796" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63258,7 +63258,7 @@
         <v>62</v>
       </c>
       <c r="V1797" s="45" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1798" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63719,7 +63719,7 @@
         <v>62</v>
       </c>
       <c r="V1815" s="45" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1816" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63891,7 +63891,7 @@
         <v>62</v>
       </c>
       <c r="V1822" s="45" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1823" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64040,7 +64040,7 @@
         <v>62</v>
       </c>
       <c r="V1828" s="45" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1829" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64213,7 +64213,7 @@
         <v>62</v>
       </c>
       <c r="V1835" s="45" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1836" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64578,7 +64578,7 @@
         <v>62</v>
       </c>
       <c r="V1850" s="45" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1851" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64767,10 +64767,10 @@
         <v>65</v>
       </c>
       <c r="S1857" s="8" t="s">
+        <v>1210</v>
+      </c>
+      <c r="T1857" s="8" t="s">
         <v>1211</v>
-      </c>
-      <c r="T1857" s="8" t="s">
-        <v>1212</v>
       </c>
       <c r="V1857" s="45"/>
     </row>
@@ -64824,7 +64824,7 @@
         <v>62</v>
       </c>
       <c r="V1859" s="45" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1860" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65085,8 +65085,8 @@
         <f t="shared" si="89"/>
         <v>101</v>
       </c>
-      <c r="N1870" s="45" t="s">
-        <v>873</v>
+      <c r="N1870" s="46" t="s">
+        <v>1231</v>
       </c>
       <c r="V1870" s="45"/>
     </row>
@@ -65110,13 +65110,13 @@
         <v>102</v>
       </c>
       <c r="N1871" s="45" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="O1871" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1871" s="45" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1872" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65139,13 +65139,13 @@
         <v>103</v>
       </c>
       <c r="N1872" s="45" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="O1872" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1872" s="45" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1873" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65168,13 +65168,13 @@
         <v>104</v>
       </c>
       <c r="N1873" s="45" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="O1873" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1873" s="45" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1874" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65248,7 +65248,7 @@
         <v>107</v>
       </c>
       <c r="N1876" s="45" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="O1876" s="8" t="s">
         <v>65</v>
@@ -65278,7 +65278,7 @@
         <v>108</v>
       </c>
       <c r="N1877" s="45" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="V1877" s="45"/>
     </row>
@@ -65305,7 +65305,7 @@
         <v>109</v>
       </c>
       <c r="N1878" s="45" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="V1878" s="45"/>
     </row>
@@ -65362,7 +65362,7 @@
         <v>111</v>
       </c>
       <c r="N1880" s="45" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="V1880" s="45"/>
     </row>
@@ -65389,7 +65389,7 @@
         <v>112</v>
       </c>
       <c r="N1881" s="45" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="V1881" s="45"/>
     </row>
@@ -65437,7 +65437,7 @@
         <v>114</v>
       </c>
       <c r="N1883" s="45" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="V1883" s="45"/>
     </row>
@@ -65461,7 +65461,7 @@
         <v>115</v>
       </c>
       <c r="N1884" s="45" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="V1884" s="45"/>
     </row>
@@ -65485,7 +65485,7 @@
         <v>116</v>
       </c>
       <c r="N1885" s="45" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="O1885" s="8" t="s">
         <v>65</v>
@@ -65512,7 +65512,7 @@
         <v>117</v>
       </c>
       <c r="N1886" s="45" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="V1886" s="45"/>
     </row>
@@ -65563,7 +65563,7 @@
         <v>119</v>
       </c>
       <c r="N1888" s="45" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="V1888" s="45"/>
     </row>
@@ -65587,7 +65587,7 @@
         <v>120</v>
       </c>
       <c r="N1889" s="45" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="V1889" s="45"/>
     </row>
@@ -65635,13 +65635,13 @@
         <v>122</v>
       </c>
       <c r="N1891" s="45" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="O1891" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1891" s="45" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1892" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65664,7 +65664,7 @@
         <v>123</v>
       </c>
       <c r="N1892" s="45" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="V1892" s="45"/>
     </row>
@@ -65712,7 +65712,7 @@
         <v>125</v>
       </c>
       <c r="N1894" s="45" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="V1894" s="45"/>
     </row>
@@ -65736,13 +65736,13 @@
         <v>126</v>
       </c>
       <c r="N1895" s="45" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="O1895" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1895" s="45" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1896" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65861,7 +65861,7 @@
         <v>131</v>
       </c>
       <c r="N1900" s="45" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="V1900" s="45"/>
     </row>
@@ -65939,7 +65939,7 @@
         <v>134</v>
       </c>
       <c r="N1903" s="45" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="V1903" s="45"/>
     </row>
@@ -65966,13 +65966,13 @@
         <v>135</v>
       </c>
       <c r="N1904" s="45" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="O1904" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1904" s="45" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1905" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66028,7 +66028,7 @@
         <v>137</v>
       </c>
       <c r="N1906" s="45" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="V1906" s="45"/>
     </row>
@@ -66154,7 +66154,7 @@
         <v>142</v>
       </c>
       <c r="N1911" s="45" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="V1911" s="45"/>
     </row>
@@ -66202,7 +66202,7 @@
         <v>144</v>
       </c>
       <c r="N1913" s="45" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="V1913" s="45"/>
     </row>
@@ -66226,13 +66226,13 @@
         <v>145</v>
       </c>
       <c r="N1914" s="45" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="O1914" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1914" s="45" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1915" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66255,13 +66255,13 @@
         <v>146</v>
       </c>
       <c r="N1915" s="45" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="O1915" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1915" s="45" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1916" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66428,7 +66428,7 @@
         <v>153</v>
       </c>
       <c r="N1922" s="45" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="V1922" s="45"/>
     </row>
@@ -66452,7 +66452,7 @@
         <v>154</v>
       </c>
       <c r="N1923" s="45" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V1923" s="45"/>
     </row>
@@ -66476,7 +66476,7 @@
         <v>155</v>
       </c>
       <c r="N1924" s="45" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="V1924" s="45"/>
     </row>
@@ -66500,7 +66500,7 @@
         <v>156</v>
       </c>
       <c r="N1925" s="45" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="V1925" s="45"/>
     </row>
@@ -66581,7 +66581,7 @@
         <v>159</v>
       </c>
       <c r="N1928" s="45" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="V1928" s="45"/>
     </row>
@@ -66635,7 +66635,7 @@
         <v>161</v>
       </c>
       <c r="N1930" s="45" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="V1930" s="45"/>
     </row>
@@ -66662,13 +66662,13 @@
         <v>162</v>
       </c>
       <c r="N1931" s="45" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="O1931" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1931" s="45" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1932" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66691,7 +66691,7 @@
         <v>163</v>
       </c>
       <c r="N1932" s="45" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V1932" s="45"/>
     </row>
@@ -66739,13 +66739,13 @@
         <v>165</v>
       </c>
       <c r="N1934" s="45" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="O1934" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1934" s="45" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1935" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66768,7 +66768,7 @@
         <v>166</v>
       </c>
       <c r="N1935" s="45" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="V1935" s="45"/>
     </row>
@@ -66822,7 +66822,7 @@
         <v>63</v>
       </c>
       <c r="V1937" s="45" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1938" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66870,7 +66870,7 @@
         <v>2</v>
       </c>
       <c r="N1939" s="45" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="V1939" s="45"/>
     </row>
@@ -66894,7 +66894,7 @@
         <v>3</v>
       </c>
       <c r="N1940" s="45" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="V1940" s="45"/>
     </row>
@@ -66918,7 +66918,7 @@
         <v>4</v>
       </c>
       <c r="N1941" s="45" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="V1941" s="45"/>
     </row>
@@ -66966,7 +66966,7 @@
         <v>6</v>
       </c>
       <c r="N1943" s="45" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="V1943" s="45"/>
     </row>
@@ -66990,7 +66990,7 @@
         <v>7</v>
       </c>
       <c r="N1944" s="45" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V1944" s="45"/>
     </row>
@@ -67014,7 +67014,7 @@
         <v>8</v>
       </c>
       <c r="N1945" s="45" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="V1945" s="45"/>
     </row>
@@ -67038,13 +67038,13 @@
         <v>9</v>
       </c>
       <c r="N1946" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="O1946" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1946" s="45" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1947" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67067,7 +67067,7 @@
         <v>10</v>
       </c>
       <c r="N1947" s="45" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="V1947" s="45"/>
     </row>
@@ -67115,7 +67115,7 @@
         <v>12</v>
       </c>
       <c r="N1949" s="45" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="V1949" s="45"/>
     </row>
@@ -67190,7 +67190,7 @@
         <v>15</v>
       </c>
       <c r="N1952" s="45" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="V1952" s="45"/>
     </row>
@@ -67214,7 +67214,7 @@
         <v>16</v>
       </c>
       <c r="N1953" s="45" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="V1953" s="45"/>
     </row>
@@ -67310,7 +67310,7 @@
         <v>20</v>
       </c>
       <c r="N1957" s="45" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="V1957" s="45"/>
     </row>
@@ -67334,7 +67334,7 @@
         <v>21</v>
       </c>
       <c r="N1958" s="45" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V1958" s="45"/>
     </row>
@@ -67364,7 +67364,7 @@
         <v>76</v>
       </c>
       <c r="T1959" s="8" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="V1959" s="45"/>
     </row>
@@ -67388,7 +67388,7 @@
         <v>23</v>
       </c>
       <c r="N1960" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="O1960" s="8" t="s">
         <v>62</v>
@@ -67396,7 +67396,7 @@
       <c r="S1960" s="8"/>
       <c r="T1960" s="8"/>
       <c r="V1960" s="45" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1961" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67419,7 +67419,7 @@
         <v>24</v>
       </c>
       <c r="N1961" s="45" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="S1961" s="8"/>
       <c r="T1961" s="8"/>
@@ -67471,7 +67471,7 @@
         <v>26</v>
       </c>
       <c r="N1963" s="45" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="S1963" s="8"/>
       <c r="T1963" s="8"/>
@@ -67552,7 +67552,7 @@
         <v>29</v>
       </c>
       <c r="N1966" s="45" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="S1966" s="8"/>
       <c r="T1966" s="8"/>
@@ -67587,10 +67587,10 @@
         <v>76</v>
       </c>
       <c r="T1967" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="V1967" s="45" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="1968" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67685,7 +67685,7 @@
         <v>34</v>
       </c>
       <c r="N1971" s="45" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="V1971" s="45"/>
     </row>
@@ -67736,7 +67736,7 @@
         <v>36</v>
       </c>
       <c r="N1973" s="45" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="V1973" s="45"/>
     </row>
@@ -67760,7 +67760,7 @@
         <v>37</v>
       </c>
       <c r="N1974" s="45" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="V1974" s="45"/>
     </row>
@@ -67784,7 +67784,7 @@
         <v>38</v>
       </c>
       <c r="N1975" s="45" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="V1975" s="45"/>
     </row>
@@ -67832,7 +67832,7 @@
         <v>40</v>
       </c>
       <c r="N1977" s="45" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="V1977" s="45"/>
     </row>
@@ -67856,7 +67856,7 @@
         <v>41</v>
       </c>
       <c r="N1978" s="45" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V1978" s="45"/>
     </row>
@@ -67880,7 +67880,7 @@
         <v>42</v>
       </c>
       <c r="N1979" s="45" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="V1979" s="45"/>
     </row>
@@ -67904,13 +67904,13 @@
         <v>43</v>
       </c>
       <c r="N1980" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="O1980" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1980" s="45" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1981" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67933,7 +67933,7 @@
         <v>44</v>
       </c>
       <c r="N1981" s="45" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V1981" s="45"/>
     </row>
@@ -67984,7 +67984,7 @@
         <v>46</v>
       </c>
       <c r="N1983" s="45" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="V1983" s="45"/>
     </row>
@@ -68008,7 +68008,7 @@
         <v>47</v>
       </c>
       <c r="N1984" s="45" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="O1984" s="8" t="s">
         <v>65</v>
@@ -68059,7 +68059,7 @@
         <v>49</v>
       </c>
       <c r="N1986" s="45" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V1986" s="45"/>
     </row>
@@ -68089,7 +68089,7 @@
         <v>76</v>
       </c>
       <c r="T1987" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="V1987" s="45"/>
     </row>
@@ -68112,13 +68112,13 @@
         <v>51</v>
       </c>
       <c r="N1988" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="O1988" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1988" s="45" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1989" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68141,7 +68141,7 @@
         <v>52</v>
       </c>
       <c r="N1989" s="45" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V1989" s="45"/>
     </row>
@@ -68192,7 +68192,7 @@
         <v>54</v>
       </c>
       <c r="N1991" s="51" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="V1991" s="45"/>
     </row>
@@ -68222,7 +68222,7 @@
         <v>76</v>
       </c>
       <c r="T1992" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="V1992" s="45"/>
     </row>
@@ -68324,7 +68324,7 @@
         <v>59</v>
       </c>
       <c r="N1996" s="45" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="V1996" s="45"/>
     </row>
@@ -68348,7 +68348,7 @@
         <v>60</v>
       </c>
       <c r="N1997" s="45" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="V1997" s="45"/>
     </row>
@@ -68372,7 +68372,7 @@
         <v>61</v>
       </c>
       <c r="N1998" s="45" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="V1998" s="45"/>
     </row>
@@ -68420,7 +68420,7 @@
         <v>63</v>
       </c>
       <c r="N2000" s="45" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="V2000" s="45"/>
     </row>
@@ -68444,7 +68444,7 @@
         <v>64</v>
       </c>
       <c r="N2001" s="45" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V2001" s="45"/>
     </row>
@@ -68468,7 +68468,7 @@
         <v>65</v>
       </c>
       <c r="N2002" s="45" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="V2002" s="45"/>
     </row>
@@ -68492,13 +68492,13 @@
         <v>66</v>
       </c>
       <c r="N2003" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="O2003" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2003" s="45" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="2004" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68521,7 +68521,7 @@
         <v>67</v>
       </c>
       <c r="N2004" s="45" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V2004" s="45"/>
     </row>
@@ -68572,7 +68572,7 @@
         <v>69</v>
       </c>
       <c r="N2006" s="45" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="V2006" s="45"/>
     </row>
@@ -68620,7 +68620,7 @@
         <v>71</v>
       </c>
       <c r="N2008" s="45" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="V2008" s="45"/>
     </row>
@@ -68695,7 +68695,7 @@
         <v>74</v>
       </c>
       <c r="N2011" s="45" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V2011" s="45"/>
     </row>
@@ -68725,7 +68725,7 @@
         <v>76</v>
       </c>
       <c r="T2012" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="V2012" s="45"/>
     </row>
@@ -68749,13 +68749,13 @@
         <v>76</v>
       </c>
       <c r="N2013" s="45" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="O2013" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2013" s="45" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="2014" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68778,7 +68778,7 @@
         <v>77</v>
       </c>
       <c r="N2014" s="45" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V2014" s="45"/>
     </row>
@@ -68829,7 +68829,7 @@
         <v>79</v>
       </c>
       <c r="N2016" s="45" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="V2016" s="45"/>
     </row>
@@ -68877,7 +68877,7 @@
         <v>81</v>
       </c>
       <c r="N2018" s="45" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="V2018" s="45"/>
     </row>
@@ -68901,13 +68901,13 @@
         <v>82</v>
       </c>
       <c r="N2019" s="45" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="O2019" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2019" s="45" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="2020" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69002,13 +69002,13 @@
         <v>86</v>
       </c>
       <c r="N2023" s="45" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="O2023" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2023" s="45" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="2024" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69055,13 +69055,13 @@
         <v>88</v>
       </c>
       <c r="N2025" s="45" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="O2025" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2025" s="45" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="2026" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69108,7 +69108,7 @@
         <v>90</v>
       </c>
       <c r="N2027" s="45" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="V2027" s="45"/>
     </row>
@@ -69156,7 +69156,7 @@
         <v>92</v>
       </c>
       <c r="N2029" s="45" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="V2029" s="45"/>
     </row>
@@ -69252,13 +69252,13 @@
         <v>96</v>
       </c>
       <c r="N2033" s="45" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="O2033" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2033" s="45" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="2034" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69311,7 +69311,7 @@
         <v>62</v>
       </c>
       <c r="V2035" s="45" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="2036" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69334,7 +69334,7 @@
         <v>99</v>
       </c>
       <c r="N2036" s="45" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="V2036" s="45"/>
     </row>
@@ -69381,13 +69381,13 @@
         <v>101</v>
       </c>
       <c r="N2038" s="45" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O2038" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2038" s="45" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="2039" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69434,7 +69434,7 @@
         <v>103</v>
       </c>
       <c r="N2040" s="45" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="V2040" s="45"/>
     </row>
@@ -69482,7 +69482,7 @@
         <v>105</v>
       </c>
       <c r="N2042" s="45" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="V2042" s="45"/>
     </row>
@@ -69602,13 +69602,13 @@
         <v>110</v>
       </c>
       <c r="N2047" s="45" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="O2047" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2047" s="45" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="2048" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69655,7 +69655,7 @@
         <v>112</v>
       </c>
       <c r="N2049" s="45" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="V2049" s="45"/>
     </row>
@@ -69703,13 +69703,13 @@
         <v>114</v>
       </c>
       <c r="N2051" s="45" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="O2051" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2051" s="45" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="2052" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69903,13 +69903,13 @@
         <v>122</v>
       </c>
       <c r="N2059" s="45" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="O2059" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2059" s="45" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="2060" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69932,13 +69932,13 @@
         <v>123</v>
       </c>
       <c r="N2060" s="45" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="O2060" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2060" s="45" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="2061" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69961,7 +69961,7 @@
         <v>124</v>
       </c>
       <c r="N2061" s="45" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="V2061" s="45"/>
     </row>
@@ -69985,7 +69985,7 @@
         <v>125</v>
       </c>
       <c r="N2062" s="45" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="V2062" s="45"/>
     </row>
@@ -70009,7 +70009,7 @@
         <v>126</v>
       </c>
       <c r="N2063" s="45" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="V2063" s="45"/>
     </row>
@@ -70105,7 +70105,7 @@
         <v>130</v>
       </c>
       <c r="N2067" s="45" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="V2067" s="45"/>
     </row>
@@ -70273,7 +70273,7 @@
         <v>137</v>
       </c>
       <c r="N2074" s="45" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="V2074" s="45"/>
     </row>
@@ -70348,13 +70348,13 @@
         <v>140</v>
       </c>
       <c r="N2077" s="45" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="O2077" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2077" s="45" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="2078" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70383,7 +70383,7 @@
         <v>62</v>
       </c>
       <c r="V2078" s="45" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="2079" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70406,7 +70406,7 @@
         <v>142</v>
       </c>
       <c r="N2079" s="45" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="V2079" s="45"/>
     </row>
@@ -70430,7 +70430,7 @@
         <v>143</v>
       </c>
       <c r="N2080" s="45" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="V2080" s="45"/>
     </row>
@@ -70478,7 +70478,7 @@
         <v>145</v>
       </c>
       <c r="N2082" s="45" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="V2082" s="45"/>
     </row>
@@ -70526,13 +70526,13 @@
         <v>147</v>
       </c>
       <c r="N2084" s="45" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="O2084" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2084" s="45" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="2085" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70555,7 +70555,7 @@
         <v>148</v>
       </c>
       <c r="N2085" s="45" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="V2085" s="45"/>
     </row>
@@ -70603,7 +70603,7 @@
         <v>150</v>
       </c>
       <c r="N2087" s="46" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="V2087" s="45"/>
     </row>
@@ -70653,7 +70653,7 @@
         <v>152</v>
       </c>
       <c r="N2089" s="45" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="V2089" s="45"/>
     </row>
@@ -70725,13 +70725,13 @@
         <v>155</v>
       </c>
       <c r="N2092" s="45" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="O2092" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2092" s="45" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="2093" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70778,7 +70778,7 @@
         <v>157</v>
       </c>
       <c r="N2094" s="45" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="V2094" s="45"/>
     </row>
@@ -70850,13 +70850,13 @@
         <v>160</v>
       </c>
       <c r="N2097" s="45" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="O2097" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2097" s="45" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="2098" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70879,7 +70879,7 @@
         <v>161</v>
       </c>
       <c r="N2098" s="45" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="V2098" s="45"/>
     </row>
@@ -70972,7 +70972,7 @@
         <v>70</v>
       </c>
       <c r="T2101" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="V2101" s="45"/>
     </row>
@@ -70999,7 +70999,7 @@
         <v>165</v>
       </c>
       <c r="N2102" s="45" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="V2102" s="45"/>
     </row>
@@ -71023,7 +71023,7 @@
         <v>166</v>
       </c>
       <c r="N2103" s="45" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="V2103" s="45"/>
     </row>
@@ -71119,13 +71119,13 @@
         <v>170</v>
       </c>
       <c r="N2107" s="45" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="O2107" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2107" s="45" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="2108" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71148,7 +71148,7 @@
         <v>171</v>
       </c>
       <c r="N2108" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="V2108" s="45"/>
     </row>
@@ -71196,13 +71196,13 @@
         <v>173</v>
       </c>
       <c r="N2110" s="45" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="O2110" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2110" s="45" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="2111" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71225,7 +71225,7 @@
         <v>174</v>
       </c>
       <c r="N2111" s="45" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="V2111" s="45"/>
     </row>
@@ -71255,10 +71255,10 @@
         <v>65</v>
       </c>
       <c r="S2112" s="8" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="T2112" s="8" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="V2112" s="45"/>
     </row>
@@ -71282,7 +71282,7 @@
         <v>176</v>
       </c>
       <c r="N2113" s="45" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="V2113" s="45"/>
     </row>
@@ -71330,13 +71330,13 @@
         <v>178</v>
       </c>
       <c r="N2115" s="45" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="O2115" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2115" s="45" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="2116" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71359,7 +71359,7 @@
         <v>179</v>
       </c>
       <c r="N2116" s="45" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="V2116" s="45"/>
     </row>
@@ -71410,7 +71410,7 @@
         <v>181</v>
       </c>
       <c r="N2118" s="45" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="V2118" s="45"/>
     </row>
@@ -71482,13 +71482,13 @@
         <v>184</v>
       </c>
       <c r="N2121" s="45" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="O2121" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2121" s="45" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="2122" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71607,7 +71607,7 @@
         <v>189</v>
       </c>
       <c r="N2126" s="45" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="O2126" s="8" t="s">
         <v>65</v>
@@ -71634,7 +71634,7 @@
         <v>190</v>
       </c>
       <c r="N2127" s="45" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="V2127" s="45"/>
     </row>
@@ -71658,13 +71658,13 @@
         <v>191</v>
       </c>
       <c r="N2128" s="45" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="O2128" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2128" s="45" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="2129" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71735,7 +71735,7 @@
         <v>194</v>
       </c>
       <c r="N2131" s="45" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="V2131" s="45"/>
     </row>
@@ -71783,7 +71783,7 @@
         <v>196</v>
       </c>
       <c r="N2133" s="45" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V2133" s="45"/>
     </row>
@@ -71807,7 +71807,7 @@
         <v>197</v>
       </c>
       <c r="N2134" s="45" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="V2134" s="45"/>
     </row>
@@ -71831,7 +71831,7 @@
         <v>198</v>
       </c>
       <c r="N2135" s="45" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="V2135" s="45"/>
     </row>
@@ -71879,7 +71879,7 @@
         <v>200</v>
       </c>
       <c r="N2137" s="46" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="V2137" s="46"/>
     </row>
@@ -71927,13 +71927,13 @@
         <v>202</v>
       </c>
       <c r="N2139" s="45" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="O2139" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2139" s="45" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="2140" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71980,7 +71980,7 @@
         <v>204</v>
       </c>
       <c r="N2141" s="45" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="V2141" s="45"/>
     </row>
@@ -72004,7 +72004,7 @@
         <v>205</v>
       </c>
       <c r="N2142" s="45" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="V2142" s="45"/>
     </row>
@@ -72028,13 +72028,13 @@
         <v>206</v>
       </c>
       <c r="N2143" s="45" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="O2143" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V2143" s="45" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="2144" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72057,7 +72057,7 @@
         <v>207</v>
       </c>
       <c r="N2144" s="45" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="V2144" s="45"/>
     </row>
@@ -72081,7 +72081,7 @@
         <v>208</v>
       </c>
       <c r="N2145" s="45" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="V2145" s="45"/>
     </row>
@@ -72105,7 +72105,7 @@
         <v>209</v>
       </c>
       <c r="N2146" s="45" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="V2146" s="45"/>
     </row>
@@ -72129,7 +72129,7 @@
         <v>210</v>
       </c>
       <c r="N2147" s="45" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="V2147" s="45"/>
     </row>
@@ -72153,7 +72153,7 @@
         <v>211</v>
       </c>
       <c r="N2148" s="45" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="V2148" s="45"/>
     </row>
@@ -72225,7 +72225,7 @@
         <v>214</v>
       </c>
       <c r="N2151" s="56" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="O2151" s="8" t="s">
         <v>62</v>
@@ -72234,7 +72234,7 @@
         <v>63</v>
       </c>
       <c r="V2151" s="45" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 01 01 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.5 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88781A54-C7E3-4EB5-9D75-C446E2AA6FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87063EA5-9FDD-43DF-AC38-435D5182044F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="1233">
   <si>
     <t>Passage</t>
   </si>
@@ -3788,6 +3788,9 @@
   </si>
   <si>
     <t xml:space="preserve">garBe#Na </t>
+  </si>
+  <si>
+    <t xml:space="preserve">catu#ShpAdaH </t>
   </si>
 </sst>
 </file>
@@ -4045,7 +4048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4252,6 +4255,27 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4535,10 +4559,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1863" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1870" sqref="N1870"/>
+      <selection pane="bottomLeft" activeCell="L468" sqref="L468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -21019,39 +21043,39 @@
       <c r="U463" s="8"/>
       <c r="V463" s="45"/>
     </row>
-    <row r="464" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D464" s="24"/>
-      <c r="I464" s="48" t="s">
+    <row r="464" spans="1:22" s="71" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D464" s="72"/>
+      <c r="I464" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="J464" s="9">
+      <c r="J464" s="74">
         <v>10</v>
       </c>
-      <c r="K464" s="6">
+      <c r="K464" s="75">
         <f t="shared" si="21"/>
         <v>463</v>
       </c>
-      <c r="L464" s="6">
+      <c r="L464" s="75">
         <f t="shared" si="22"/>
         <v>41</v>
       </c>
-      <c r="M464" s="6">
+      <c r="M464" s="75">
         <f t="shared" si="23"/>
         <v>91</v>
       </c>
-      <c r="N464" s="45" t="s">
+      <c r="N464" s="76" t="s">
         <v>348</v>
       </c>
-      <c r="O464" s="8" t="s">
+      <c r="O464" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="P464" s="8"/>
-      <c r="Q464" s="8"/>
-      <c r="R464" s="8"/>
-      <c r="S464" s="8"/>
-      <c r="T464" s="8"/>
-      <c r="U464" s="8"/>
-      <c r="V464" s="45" t="s">
+      <c r="P464" s="77"/>
+      <c r="Q464" s="77"/>
+      <c r="R464" s="77"/>
+      <c r="S464" s="77"/>
+      <c r="T464" s="77"/>
+      <c r="U464" s="77"/>
+      <c r="V464" s="76" t="s">
         <v>1016</v>
       </c>
     </row>
@@ -21173,8 +21197,8 @@
         <f t="shared" si="23"/>
         <v>95</v>
       </c>
-      <c r="N468" s="45" t="s">
-        <v>350</v>
+      <c r="N468" s="46" t="s">
+        <v>1232</v>
       </c>
       <c r="O468" s="8" t="s">
         <v>62</v>

</xml_diff>